<commit_message>
Holden, BOS and History
</commit_message>
<xml_diff>
--- a/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
+++ b/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="539">
   <si>
     <t>TITAN</t>
   </si>
@@ -1668,6 +1668,21 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>461</t>
+  </si>
+  <si>
+    <t>463</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>462</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1819,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1827,12 +1842,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1900,6 +1952,15 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2191,7 +2252,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="AL3" sqref="AL3"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2554,9 @@
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="26" t="s">
+        <v>538</v>
+      </c>
       <c r="B3" s="6" t="b">
         <v>1</v>
       </c>
@@ -2611,11 +2674,11 @@
         <v>19</v>
       </c>
       <c r="AR3" s="22" t="s">
-        <v>38</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="6" t="b">
         <v>1</v>
       </c>
@@ -2737,7 +2800,7 @@
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="6" t="b">
         <v>1</v>
       </c>
@@ -2855,11 +2918,11 @@
         <v>19</v>
       </c>
       <c r="AR5" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="6" t="b">
         <v>1</v>
       </c>
@@ -2977,7 +3040,7 @@
         <v>19</v>
       </c>
       <c r="AR6" s="22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
@@ -3099,7 +3162,7 @@
         <v>19</v>
       </c>
       <c r="AR7" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
@@ -3147,7 +3210,7 @@
       <c r="AP8" s="19"/>
       <c r="AQ8" s="19"/>
       <c r="AR8" s="22" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
@@ -3195,7 +3258,7 @@
       <c r="AP9" s="19"/>
       <c r="AQ9" s="19"/>
       <c r="AR9" s="22" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
@@ -3243,7 +3306,7 @@
       <c r="AP10" s="19"/>
       <c r="AQ10" s="19"/>
       <c r="AR10" s="22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
@@ -3291,7 +3354,7 @@
       <c r="AP11" s="19"/>
       <c r="AQ11" s="19"/>
       <c r="AR11" s="22" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
@@ -3339,7 +3402,7 @@
       <c r="AP12" s="19"/>
       <c r="AQ12" s="19"/>
       <c r="AR12" s="22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
@@ -3387,7 +3450,7 @@
       <c r="AP13" s="19"/>
       <c r="AQ13" s="19"/>
       <c r="AR13" s="22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
@@ -3435,7 +3498,7 @@
       <c r="AP14" s="19"/>
       <c r="AQ14" s="19"/>
       <c r="AR14" s="22" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
@@ -3483,7 +3546,7 @@
       <c r="AP15" s="19"/>
       <c r="AQ15" s="19"/>
       <c r="AR15" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
@@ -3531,7 +3594,7 @@
       <c r="AP16" s="19"/>
       <c r="AQ16" s="19"/>
       <c r="AR16" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
@@ -3579,7 +3642,7 @@
       <c r="AP17" s="19"/>
       <c r="AQ17" s="19"/>
       <c r="AR17" s="22" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.25">
@@ -3627,7 +3690,7 @@
       <c r="AP18" s="19"/>
       <c r="AQ18" s="19"/>
       <c r="AR18" s="22" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:44" x14ac:dyDescent="0.25">
@@ -3675,7 +3738,7 @@
       <c r="AP19" s="19"/>
       <c r="AQ19" s="19"/>
       <c r="AR19" s="22" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:44" x14ac:dyDescent="0.25">
@@ -3723,7 +3786,7 @@
       <c r="AP20" s="19"/>
       <c r="AQ20" s="19"/>
       <c r="AR20" s="22" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.25">
@@ -3771,7 +3834,7 @@
       <c r="AP21" s="19"/>
       <c r="AQ21" s="19"/>
       <c r="AR21" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.25">
@@ -3819,7 +3882,7 @@
       <c r="AP22" s="19"/>
       <c r="AQ22" s="19"/>
       <c r="AR22" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.25">
@@ -3867,7 +3930,7 @@
       <c r="AP23" s="19"/>
       <c r="AQ23" s="19"/>
       <c r="AR23" s="22" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.25">
@@ -3915,7 +3978,7 @@
       <c r="AP24" s="19"/>
       <c r="AQ24" s="19"/>
       <c r="AR24" s="22" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.25">
@@ -3963,7 +4026,7 @@
       <c r="AP25" s="19"/>
       <c r="AQ25" s="19"/>
       <c r="AR25" s="22" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.25">
@@ -4011,7 +4074,7 @@
       <c r="AP26" s="19"/>
       <c r="AQ26" s="19"/>
       <c r="AR26" s="22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.25">
@@ -4059,7 +4122,7 @@
       <c r="AP27" s="19"/>
       <c r="AQ27" s="19"/>
       <c r="AR27" s="22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.25">
@@ -4107,7 +4170,7 @@
       <c r="AP28" s="19"/>
       <c r="AQ28" s="19"/>
       <c r="AR28" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:44" x14ac:dyDescent="0.25">
@@ -4155,7 +4218,7 @@
       <c r="AP29" s="19"/>
       <c r="AQ29" s="19"/>
       <c r="AR29" s="22" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.25">
@@ -4203,7 +4266,7 @@
       <c r="AP30" s="19"/>
       <c r="AQ30" s="19"/>
       <c r="AR30" s="22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:44" x14ac:dyDescent="0.25">
@@ -4251,7 +4314,7 @@
       <c r="AP31" s="19"/>
       <c r="AQ31" s="19"/>
       <c r="AR31" s="22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.25">
@@ -4299,7 +4362,7 @@
       <c r="AP32" s="19"/>
       <c r="AQ32" s="19"/>
       <c r="AR32" s="22" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:44" x14ac:dyDescent="0.25">
@@ -4347,7 +4410,7 @@
       <c r="AP33" s="19"/>
       <c r="AQ33" s="19"/>
       <c r="AR33" s="22" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.25">
@@ -4395,7 +4458,7 @@
       <c r="AP34" s="19"/>
       <c r="AQ34" s="19"/>
       <c r="AR34" s="22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:44" x14ac:dyDescent="0.25">
@@ -4443,7 +4506,7 @@
       <c r="AP35" s="19"/>
       <c r="AQ35" s="19"/>
       <c r="AR35" s="22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.25">
@@ -4491,7 +4554,7 @@
       <c r="AP36" s="19"/>
       <c r="AQ36" s="19"/>
       <c r="AR36" s="22" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.25">
@@ -4539,7 +4602,7 @@
       <c r="AP37" s="19"/>
       <c r="AQ37" s="19"/>
       <c r="AR37" s="22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:44" x14ac:dyDescent="0.25">
@@ -4587,7 +4650,7 @@
       <c r="AP38" s="19"/>
       <c r="AQ38" s="19"/>
       <c r="AR38" s="22" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:44" x14ac:dyDescent="0.25">
@@ -4635,7 +4698,7 @@
       <c r="AP39" s="19"/>
       <c r="AQ39" s="19"/>
       <c r="AR39" s="22" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:44" x14ac:dyDescent="0.25">
@@ -4683,7 +4746,7 @@
       <c r="AP40" s="19"/>
       <c r="AQ40" s="19"/>
       <c r="AR40" s="22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.25">
@@ -4731,7 +4794,7 @@
       <c r="AP41" s="19"/>
       <c r="AQ41" s="19"/>
       <c r="AR41" s="22" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:44" x14ac:dyDescent="0.25">
@@ -4779,7 +4842,7 @@
       <c r="AP42" s="19"/>
       <c r="AQ42" s="19"/>
       <c r="AR42" s="22" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:44" x14ac:dyDescent="0.25">
@@ -4827,7 +4890,7 @@
       <c r="AP43" s="19"/>
       <c r="AQ43" s="19"/>
       <c r="AR43" s="22" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:44" x14ac:dyDescent="0.25">
@@ -4875,7 +4938,7 @@
       <c r="AP44" s="19"/>
       <c r="AQ44" s="19"/>
       <c r="AR44" s="22" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:44" x14ac:dyDescent="0.25">
@@ -4923,7 +4986,7 @@
       <c r="AP45" s="19"/>
       <c r="AQ45" s="19"/>
       <c r="AR45" s="22" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:44" x14ac:dyDescent="0.25">
@@ -4971,7 +5034,7 @@
       <c r="AP46" s="19"/>
       <c r="AQ46" s="19"/>
       <c r="AR46" s="22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:44" x14ac:dyDescent="0.25">
@@ -5019,7 +5082,7 @@
       <c r="AP47" s="19"/>
       <c r="AQ47" s="19"/>
       <c r="AR47" s="22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:44" x14ac:dyDescent="0.25">
@@ -5067,7 +5130,7 @@
       <c r="AP48" s="19"/>
       <c r="AQ48" s="19"/>
       <c r="AR48" s="22" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:44" x14ac:dyDescent="0.25">
@@ -5115,7 +5178,7 @@
       <c r="AP49" s="19"/>
       <c r="AQ49" s="19"/>
       <c r="AR49" s="22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:44" x14ac:dyDescent="0.25">
@@ -5163,7 +5226,7 @@
       <c r="AP50" s="19"/>
       <c r="AQ50" s="19"/>
       <c r="AR50" s="22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:44" x14ac:dyDescent="0.25">
@@ -5211,7 +5274,7 @@
       <c r="AP51" s="19"/>
       <c r="AQ51" s="19"/>
       <c r="AR51" s="22" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:44" x14ac:dyDescent="0.25">
@@ -5259,7 +5322,7 @@
       <c r="AP52" s="19"/>
       <c r="AQ52" s="19"/>
       <c r="AR52" s="22" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:44" x14ac:dyDescent="0.25">
@@ -5307,7 +5370,7 @@
       <c r="AP53" s="19"/>
       <c r="AQ53" s="19"/>
       <c r="AR53" s="22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:44" x14ac:dyDescent="0.25">
@@ -5355,7 +5418,7 @@
       <c r="AP54" s="19"/>
       <c r="AQ54" s="19"/>
       <c r="AR54" s="22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:44" x14ac:dyDescent="0.25">
@@ -5403,7 +5466,7 @@
       <c r="AP55" s="19"/>
       <c r="AQ55" s="19"/>
       <c r="AR55" s="22" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:44" x14ac:dyDescent="0.25">
@@ -5451,7 +5514,7 @@
       <c r="AP56" s="19"/>
       <c r="AQ56" s="19"/>
       <c r="AR56" s="22" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:44" x14ac:dyDescent="0.25">
@@ -5499,7 +5562,7 @@
       <c r="AP57" s="19"/>
       <c r="AQ57" s="19"/>
       <c r="AR57" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:44" x14ac:dyDescent="0.25">
@@ -5547,7 +5610,7 @@
       <c r="AP58" s="19"/>
       <c r="AQ58" s="19"/>
       <c r="AR58" s="22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:44" x14ac:dyDescent="0.25">
@@ -5595,7 +5658,7 @@
       <c r="AP59" s="19"/>
       <c r="AQ59" s="19"/>
       <c r="AR59" s="22" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:44" x14ac:dyDescent="0.25">
@@ -5643,7 +5706,7 @@
       <c r="AP60" s="19"/>
       <c r="AQ60" s="19"/>
       <c r="AR60" s="22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:44" x14ac:dyDescent="0.25">
@@ -5691,7 +5754,7 @@
       <c r="AP61" s="19"/>
       <c r="AQ61" s="19"/>
       <c r="AR61" s="22" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:44" x14ac:dyDescent="0.25">
@@ -5739,7 +5802,7 @@
       <c r="AP62" s="19"/>
       <c r="AQ62" s="19"/>
       <c r="AR62" s="22" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:44" x14ac:dyDescent="0.25">
@@ -5787,7 +5850,7 @@
       <c r="AP63" s="19"/>
       <c r="AQ63" s="19"/>
       <c r="AR63" s="22" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:44" x14ac:dyDescent="0.25">
@@ -5835,7 +5898,7 @@
       <c r="AP64" s="19"/>
       <c r="AQ64" s="19"/>
       <c r="AR64" s="22" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:44" x14ac:dyDescent="0.25">
@@ -5883,7 +5946,7 @@
       <c r="AP65" s="19"/>
       <c r="AQ65" s="19"/>
       <c r="AR65" s="22" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.25">
@@ -5931,7 +5994,7 @@
       <c r="AP66" s="19"/>
       <c r="AQ66" s="19"/>
       <c r="AR66" s="22" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.25">
@@ -5979,7 +6042,7 @@
       <c r="AP67" s="19"/>
       <c r="AQ67" s="19"/>
       <c r="AR67" s="22" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.25">
@@ -6027,7 +6090,7 @@
       <c r="AP68" s="19"/>
       <c r="AQ68" s="19"/>
       <c r="AR68" s="22" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.25">
@@ -6075,7 +6138,7 @@
       <c r="AP69" s="19"/>
       <c r="AQ69" s="19"/>
       <c r="AR69" s="22" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:44" x14ac:dyDescent="0.25">
@@ -6123,7 +6186,7 @@
       <c r="AP70" s="19"/>
       <c r="AQ70" s="19"/>
       <c r="AR70" s="22" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.25">
@@ -6171,7 +6234,7 @@
       <c r="AP71" s="19"/>
       <c r="AQ71" s="19"/>
       <c r="AR71" s="22" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.25">
@@ -6219,7 +6282,7 @@
       <c r="AP72" s="19"/>
       <c r="AQ72" s="19"/>
       <c r="AR72" s="22" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:44" x14ac:dyDescent="0.25">
@@ -6267,7 +6330,7 @@
       <c r="AP73" s="19"/>
       <c r="AQ73" s="19"/>
       <c r="AR73" s="22" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:44" x14ac:dyDescent="0.25">
@@ -6315,7 +6378,7 @@
       <c r="AP74" s="19"/>
       <c r="AQ74" s="19"/>
       <c r="AR74" s="22" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.25">
@@ -6363,7 +6426,7 @@
       <c r="AP75" s="19"/>
       <c r="AQ75" s="19"/>
       <c r="AR75" s="22" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.25">
@@ -6411,7 +6474,7 @@
       <c r="AP76" s="19"/>
       <c r="AQ76" s="19"/>
       <c r="AR76" s="22" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:44" x14ac:dyDescent="0.25">
@@ -6459,7 +6522,7 @@
       <c r="AP77" s="19"/>
       <c r="AQ77" s="19"/>
       <c r="AR77" s="22" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:44" x14ac:dyDescent="0.25">
@@ -6507,7 +6570,7 @@
       <c r="AP78" s="19"/>
       <c r="AQ78" s="19"/>
       <c r="AR78" s="22" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.25">
@@ -6555,7 +6618,7 @@
       <c r="AP79" s="19"/>
       <c r="AQ79" s="19"/>
       <c r="AR79" s="22" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:44" x14ac:dyDescent="0.25">
@@ -6603,7 +6666,7 @@
       <c r="AP80" s="19"/>
       <c r="AQ80" s="19"/>
       <c r="AR80" s="22" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:44" x14ac:dyDescent="0.25">
@@ -6651,7 +6714,7 @@
       <c r="AP81" s="19"/>
       <c r="AQ81" s="19"/>
       <c r="AR81" s="22" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:44" x14ac:dyDescent="0.25">
@@ -6699,7 +6762,7 @@
       <c r="AP82" s="19"/>
       <c r="AQ82" s="19"/>
       <c r="AR82" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:44" x14ac:dyDescent="0.25">
@@ -6747,7 +6810,7 @@
       <c r="AP83" s="19"/>
       <c r="AQ83" s="19"/>
       <c r="AR83" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:44" x14ac:dyDescent="0.25">
@@ -6795,7 +6858,7 @@
       <c r="AP84" s="19"/>
       <c r="AQ84" s="19"/>
       <c r="AR84" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:44" x14ac:dyDescent="0.25">
@@ -6843,7 +6906,7 @@
       <c r="AP85" s="19"/>
       <c r="AQ85" s="19"/>
       <c r="AR85" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:44" x14ac:dyDescent="0.25">
@@ -6891,7 +6954,7 @@
       <c r="AP86" s="19"/>
       <c r="AQ86" s="19"/>
       <c r="AR86" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:44" x14ac:dyDescent="0.25">
@@ -6939,7 +7002,7 @@
       <c r="AP87" s="19"/>
       <c r="AQ87" s="19"/>
       <c r="AR87" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:44" x14ac:dyDescent="0.25">
@@ -6987,7 +7050,7 @@
       <c r="AP88" s="19"/>
       <c r="AQ88" s="19"/>
       <c r="AR88" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:44" x14ac:dyDescent="0.25">
@@ -7035,7 +7098,7 @@
       <c r="AP89" s="19"/>
       <c r="AQ89" s="19"/>
       <c r="AR89" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:44" x14ac:dyDescent="0.25">
@@ -7083,7 +7146,7 @@
       <c r="AP90" s="19"/>
       <c r="AQ90" s="19"/>
       <c r="AR90" s="22" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:44" x14ac:dyDescent="0.25">
@@ -7131,7 +7194,7 @@
       <c r="AP91" s="19"/>
       <c r="AQ91" s="19"/>
       <c r="AR91" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="92" spans="1:44" x14ac:dyDescent="0.25">
@@ -7179,7 +7242,7 @@
       <c r="AP92" s="19"/>
       <c r="AQ92" s="19"/>
       <c r="AR92" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:44" x14ac:dyDescent="0.25">
@@ -7227,7 +7290,7 @@
       <c r="AP93" s="19"/>
       <c r="AQ93" s="19"/>
       <c r="AR93" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="94" spans="1:44" x14ac:dyDescent="0.25">
@@ -7275,7 +7338,7 @@
       <c r="AP94" s="19"/>
       <c r="AQ94" s="19"/>
       <c r="AR94" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="95" spans="1:44" x14ac:dyDescent="0.25">
@@ -7323,7 +7386,7 @@
       <c r="AP95" s="19"/>
       <c r="AQ95" s="19"/>
       <c r="AR95" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="96" spans="1:44" x14ac:dyDescent="0.25">
@@ -7371,7 +7434,7 @@
       <c r="AP96" s="19"/>
       <c r="AQ96" s="19"/>
       <c r="AR96" s="22" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="97" spans="1:44" x14ac:dyDescent="0.25">
@@ -7419,7 +7482,7 @@
       <c r="AP97" s="19"/>
       <c r="AQ97" s="19"/>
       <c r="AR97" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:44" x14ac:dyDescent="0.25">
@@ -7467,7 +7530,7 @@
       <c r="AP98" s="19"/>
       <c r="AQ98" s="19"/>
       <c r="AR98" s="22" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="99" spans="1:44" x14ac:dyDescent="0.25">
@@ -7515,7 +7578,7 @@
       <c r="AP99" s="19"/>
       <c r="AQ99" s="19"/>
       <c r="AR99" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="100" spans="1:44" x14ac:dyDescent="0.25">
@@ -7563,7 +7626,7 @@
       <c r="AP100" s="19"/>
       <c r="AQ100" s="19"/>
       <c r="AR100" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="101" spans="1:44" x14ac:dyDescent="0.25">
@@ -7611,7 +7674,7 @@
       <c r="AP101" s="19"/>
       <c r="AQ101" s="19"/>
       <c r="AR101" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="102" spans="1:44" x14ac:dyDescent="0.25">
@@ -7659,7 +7722,7 @@
       <c r="AP102" s="19"/>
       <c r="AQ102" s="19"/>
       <c r="AR102" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="103" spans="1:44" x14ac:dyDescent="0.25">
@@ -7707,7 +7770,7 @@
       <c r="AP103" s="19"/>
       <c r="AQ103" s="19"/>
       <c r="AR103" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="1:44" x14ac:dyDescent="0.25">
@@ -7755,7 +7818,7 @@
       <c r="AP104" s="19"/>
       <c r="AQ104" s="19"/>
       <c r="AR104" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:44" x14ac:dyDescent="0.25">
@@ -7803,7 +7866,7 @@
       <c r="AP105" s="19"/>
       <c r="AQ105" s="19"/>
       <c r="AR105" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="1:44" x14ac:dyDescent="0.25">
@@ -7851,7 +7914,7 @@
       <c r="AP106" s="19"/>
       <c r="AQ106" s="19"/>
       <c r="AR106" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:44" x14ac:dyDescent="0.25">
@@ -7899,7 +7962,7 @@
       <c r="AP107" s="19"/>
       <c r="AQ107" s="19"/>
       <c r="AR107" s="22" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="108" spans="1:44" x14ac:dyDescent="0.25">
@@ -7947,7 +8010,7 @@
       <c r="AP108" s="19"/>
       <c r="AQ108" s="19"/>
       <c r="AR108" s="22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="109" spans="1:44" x14ac:dyDescent="0.25">
@@ -7995,7 +8058,7 @@
       <c r="AP109" s="19"/>
       <c r="AQ109" s="19"/>
       <c r="AR109" s="22" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="110" spans="1:44" x14ac:dyDescent="0.25">
@@ -8043,7 +8106,7 @@
       <c r="AP110" s="19"/>
       <c r="AQ110" s="19"/>
       <c r="AR110" s="22" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="111" spans="1:44" x14ac:dyDescent="0.25">
@@ -8091,7 +8154,7 @@
       <c r="AP111" s="19"/>
       <c r="AQ111" s="19"/>
       <c r="AR111" s="22" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:44" x14ac:dyDescent="0.25">
@@ -8139,7 +8202,7 @@
       <c r="AP112" s="19"/>
       <c r="AQ112" s="19"/>
       <c r="AR112" s="22" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113" spans="1:44" x14ac:dyDescent="0.25">
@@ -8187,7 +8250,7 @@
       <c r="AP113" s="19"/>
       <c r="AQ113" s="19"/>
       <c r="AR113" s="22" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114" spans="1:44" x14ac:dyDescent="0.25">
@@ -8235,7 +8298,7 @@
       <c r="AP114" s="19"/>
       <c r="AQ114" s="19"/>
       <c r="AR114" s="22" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:44" x14ac:dyDescent="0.25">
@@ -8283,7 +8346,7 @@
       <c r="AP115" s="19"/>
       <c r="AQ115" s="19"/>
       <c r="AR115" s="22" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:44" x14ac:dyDescent="0.25">
@@ -8331,7 +8394,7 @@
       <c r="AP116" s="19"/>
       <c r="AQ116" s="19"/>
       <c r="AR116" s="22" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="117" spans="1:44" x14ac:dyDescent="0.25">
@@ -8379,7 +8442,7 @@
       <c r="AP117" s="19"/>
       <c r="AQ117" s="19"/>
       <c r="AR117" s="22" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="118" spans="1:44" x14ac:dyDescent="0.25">
@@ -8427,7 +8490,7 @@
       <c r="AP118" s="19"/>
       <c r="AQ118" s="19"/>
       <c r="AR118" s="22" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="119" spans="1:44" x14ac:dyDescent="0.25">
@@ -8475,7 +8538,7 @@
       <c r="AP119" s="19"/>
       <c r="AQ119" s="19"/>
       <c r="AR119" s="22" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="120" spans="1:44" x14ac:dyDescent="0.25">
@@ -8523,7 +8586,7 @@
       <c r="AP120" s="19"/>
       <c r="AQ120" s="19"/>
       <c r="AR120" s="22" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="121" spans="1:44" x14ac:dyDescent="0.25">
@@ -8571,7 +8634,7 @@
       <c r="AP121" s="19"/>
       <c r="AQ121" s="19"/>
       <c r="AR121" s="22" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="122" spans="1:44" x14ac:dyDescent="0.25">
@@ -8619,7 +8682,7 @@
       <c r="AP122" s="19"/>
       <c r="AQ122" s="19"/>
       <c r="AR122" s="22" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="123" spans="1:44" x14ac:dyDescent="0.25">
@@ -8667,7 +8730,7 @@
       <c r="AP123" s="19"/>
       <c r="AQ123" s="19"/>
       <c r="AR123" s="22" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="124" spans="1:44" x14ac:dyDescent="0.25">
@@ -8715,7 +8778,7 @@
       <c r="AP124" s="19"/>
       <c r="AQ124" s="19"/>
       <c r="AR124" s="22" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="125" spans="1:44" x14ac:dyDescent="0.25">
@@ -8763,7 +8826,7 @@
       <c r="AP125" s="19"/>
       <c r="AQ125" s="19"/>
       <c r="AR125" s="22" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="126" spans="1:44" x14ac:dyDescent="0.25">
@@ -8811,7 +8874,7 @@
       <c r="AP126" s="19"/>
       <c r="AQ126" s="19"/>
       <c r="AR126" s="22" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="127" spans="1:44" x14ac:dyDescent="0.25">
@@ -8859,7 +8922,7 @@
       <c r="AP127" s="19"/>
       <c r="AQ127" s="19"/>
       <c r="AR127" s="22" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="128" spans="1:44" x14ac:dyDescent="0.25">
@@ -8907,7 +8970,7 @@
       <c r="AP128" s="19"/>
       <c r="AQ128" s="19"/>
       <c r="AR128" s="22" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="129" spans="1:44" x14ac:dyDescent="0.25">
@@ -8955,7 +9018,7 @@
       <c r="AP129" s="19"/>
       <c r="AQ129" s="19"/>
       <c r="AR129" s="22" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="130" spans="1:44" x14ac:dyDescent="0.25">
@@ -9003,7 +9066,7 @@
       <c r="AP130" s="19"/>
       <c r="AQ130" s="19"/>
       <c r="AR130" s="22" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="131" spans="1:44" x14ac:dyDescent="0.25">
@@ -9051,7 +9114,7 @@
       <c r="AP131" s="19"/>
       <c r="AQ131" s="19"/>
       <c r="AR131" s="22" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="132" spans="1:44" x14ac:dyDescent="0.25">
@@ -9099,7 +9162,7 @@
       <c r="AP132" s="19"/>
       <c r="AQ132" s="19"/>
       <c r="AR132" s="22" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="133" spans="1:44" x14ac:dyDescent="0.25">
@@ -9147,7 +9210,7 @@
       <c r="AP133" s="19"/>
       <c r="AQ133" s="19"/>
       <c r="AR133" s="22" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="134" spans="1:44" x14ac:dyDescent="0.25">
@@ -9195,7 +9258,7 @@
       <c r="AP134" s="19"/>
       <c r="AQ134" s="19"/>
       <c r="AR134" s="22" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="135" spans="1:44" x14ac:dyDescent="0.25">
@@ -9243,7 +9306,7 @@
       <c r="AP135" s="19"/>
       <c r="AQ135" s="19"/>
       <c r="AR135" s="22" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="136" spans="1:44" x14ac:dyDescent="0.25">
@@ -9291,7 +9354,7 @@
       <c r="AP136" s="19"/>
       <c r="AQ136" s="19"/>
       <c r="AR136" s="22" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="137" spans="1:44" x14ac:dyDescent="0.25">
@@ -9339,7 +9402,7 @@
       <c r="AP137" s="19"/>
       <c r="AQ137" s="19"/>
       <c r="AR137" s="22" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="138" spans="1:44" x14ac:dyDescent="0.25">
@@ -9387,7 +9450,7 @@
       <c r="AP138" s="19"/>
       <c r="AQ138" s="19"/>
       <c r="AR138" s="22" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="139" spans="1:44" x14ac:dyDescent="0.25">
@@ -9435,7 +9498,7 @@
       <c r="AP139" s="19"/>
       <c r="AQ139" s="19"/>
       <c r="AR139" s="22" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="140" spans="1:44" x14ac:dyDescent="0.25">
@@ -9483,7 +9546,7 @@
       <c r="AP140" s="19"/>
       <c r="AQ140" s="19"/>
       <c r="AR140" s="22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="141" spans="1:44" x14ac:dyDescent="0.25">
@@ -9531,7 +9594,7 @@
       <c r="AP141" s="19"/>
       <c r="AQ141" s="19"/>
       <c r="AR141" s="22" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="142" spans="1:44" x14ac:dyDescent="0.25">
@@ -9579,7 +9642,7 @@
       <c r="AP142" s="19"/>
       <c r="AQ142" s="19"/>
       <c r="AR142" s="22" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="143" spans="1:44" x14ac:dyDescent="0.25">
@@ -9627,7 +9690,7 @@
       <c r="AP143" s="19"/>
       <c r="AQ143" s="19"/>
       <c r="AR143" s="22" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="144" spans="1:44" x14ac:dyDescent="0.25">
@@ -9675,7 +9738,7 @@
       <c r="AP144" s="19"/>
       <c r="AQ144" s="19"/>
       <c r="AR144" s="22" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="145" spans="1:44" x14ac:dyDescent="0.25">
@@ -9723,7 +9786,7 @@
       <c r="AP145" s="19"/>
       <c r="AQ145" s="19"/>
       <c r="AR145" s="22" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="146" spans="1:44" x14ac:dyDescent="0.25">
@@ -9771,7 +9834,7 @@
       <c r="AP146" s="19"/>
       <c r="AQ146" s="19"/>
       <c r="AR146" s="22" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="147" spans="1:44" x14ac:dyDescent="0.25">
@@ -9819,7 +9882,7 @@
       <c r="AP147" s="19"/>
       <c r="AQ147" s="19"/>
       <c r="AR147" s="22" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="148" spans="1:44" x14ac:dyDescent="0.25">
@@ -9867,7 +9930,7 @@
       <c r="AP148" s="19"/>
       <c r="AQ148" s="19"/>
       <c r="AR148" s="22" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="149" spans="1:44" x14ac:dyDescent="0.25">
@@ -9915,7 +9978,7 @@
       <c r="AP149" s="19"/>
       <c r="AQ149" s="19"/>
       <c r="AR149" s="22" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="150" spans="1:44" x14ac:dyDescent="0.25">
@@ -9963,7 +10026,7 @@
       <c r="AP150" s="19"/>
       <c r="AQ150" s="19"/>
       <c r="AR150" s="22" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="151" spans="1:44" x14ac:dyDescent="0.25">
@@ -10011,7 +10074,7 @@
       <c r="AP151" s="19"/>
       <c r="AQ151" s="19"/>
       <c r="AR151" s="22" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="152" spans="1:44" x14ac:dyDescent="0.25">
@@ -10059,7 +10122,7 @@
       <c r="AP152" s="19"/>
       <c r="AQ152" s="19"/>
       <c r="AR152" s="22" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="153" spans="1:44" x14ac:dyDescent="0.25">
@@ -10107,7 +10170,7 @@
       <c r="AP153" s="19"/>
       <c r="AQ153" s="19"/>
       <c r="AR153" s="22" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="154" spans="1:44" x14ac:dyDescent="0.25">
@@ -10155,7 +10218,7 @@
       <c r="AP154" s="19"/>
       <c r="AQ154" s="19"/>
       <c r="AR154" s="22" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="155" spans="1:44" x14ac:dyDescent="0.25">
@@ -10203,7 +10266,7 @@
       <c r="AP155" s="19"/>
       <c r="AQ155" s="19"/>
       <c r="AR155" s="22" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="156" spans="1:44" x14ac:dyDescent="0.25">
@@ -10251,7 +10314,7 @@
       <c r="AP156" s="19"/>
       <c r="AQ156" s="19"/>
       <c r="AR156" s="22" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="157" spans="1:44" x14ac:dyDescent="0.25">
@@ -10299,7 +10362,7 @@
       <c r="AP157" s="19"/>
       <c r="AQ157" s="19"/>
       <c r="AR157" s="22" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="158" spans="1:44" x14ac:dyDescent="0.25">
@@ -10347,7 +10410,7 @@
       <c r="AP158" s="19"/>
       <c r="AQ158" s="19"/>
       <c r="AR158" s="22" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="159" spans="1:44" x14ac:dyDescent="0.25">
@@ -10395,7 +10458,7 @@
       <c r="AP159" s="19"/>
       <c r="AQ159" s="19"/>
       <c r="AR159" s="22" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="160" spans="1:44" x14ac:dyDescent="0.25">
@@ -10443,7 +10506,7 @@
       <c r="AP160" s="19"/>
       <c r="AQ160" s="19"/>
       <c r="AR160" s="22" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="161" spans="1:44" x14ac:dyDescent="0.25">
@@ -10491,7 +10554,7 @@
       <c r="AP161" s="19"/>
       <c r="AQ161" s="19"/>
       <c r="AR161" s="22" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="162" spans="1:44" x14ac:dyDescent="0.25">
@@ -10539,7 +10602,7 @@
       <c r="AP162" s="19"/>
       <c r="AQ162" s="19"/>
       <c r="AR162" s="22" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="163" spans="1:44" x14ac:dyDescent="0.25">
@@ -10587,7 +10650,7 @@
       <c r="AP163" s="19"/>
       <c r="AQ163" s="19"/>
       <c r="AR163" s="22" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="164" spans="1:44" x14ac:dyDescent="0.25">
@@ -10635,7 +10698,7 @@
       <c r="AP164" s="19"/>
       <c r="AQ164" s="19"/>
       <c r="AR164" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="165" spans="1:44" x14ac:dyDescent="0.25">
@@ -10683,7 +10746,7 @@
       <c r="AP165" s="19"/>
       <c r="AQ165" s="19"/>
       <c r="AR165" s="22" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:44" x14ac:dyDescent="0.25">
@@ -10731,7 +10794,7 @@
       <c r="AP166" s="19"/>
       <c r="AQ166" s="19"/>
       <c r="AR166" s="22" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="167" spans="1:44" x14ac:dyDescent="0.25">
@@ -10779,7 +10842,7 @@
       <c r="AP167" s="19"/>
       <c r="AQ167" s="19"/>
       <c r="AR167" s="22" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="168" spans="1:44" x14ac:dyDescent="0.25">
@@ -10827,7 +10890,7 @@
       <c r="AP168" s="19"/>
       <c r="AQ168" s="19"/>
       <c r="AR168" s="22" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="169" spans="1:44" x14ac:dyDescent="0.25">
@@ -10875,7 +10938,7 @@
       <c r="AP169" s="19"/>
       <c r="AQ169" s="19"/>
       <c r="AR169" s="22" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="170" spans="1:44" x14ac:dyDescent="0.25">
@@ -10923,7 +10986,7 @@
       <c r="AP170" s="19"/>
       <c r="AQ170" s="19"/>
       <c r="AR170" s="22" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="171" spans="1:44" x14ac:dyDescent="0.25">
@@ -10971,7 +11034,7 @@
       <c r="AP171" s="19"/>
       <c r="AQ171" s="19"/>
       <c r="AR171" s="22" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="172" spans="1:44" x14ac:dyDescent="0.25">
@@ -11019,7 +11082,7 @@
       <c r="AP172" s="19"/>
       <c r="AQ172" s="19"/>
       <c r="AR172" s="22" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="173" spans="1:44" x14ac:dyDescent="0.25">
@@ -11067,7 +11130,7 @@
       <c r="AP173" s="19"/>
       <c r="AQ173" s="19"/>
       <c r="AR173" s="22" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="174" spans="1:44" x14ac:dyDescent="0.25">
@@ -11115,7 +11178,7 @@
       <c r="AP174" s="19"/>
       <c r="AQ174" s="19"/>
       <c r="AR174" s="22" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="175" spans="1:44" x14ac:dyDescent="0.25">
@@ -11163,7 +11226,7 @@
       <c r="AP175" s="19"/>
       <c r="AQ175" s="19"/>
       <c r="AR175" s="22" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="176" spans="1:44" x14ac:dyDescent="0.25">
@@ -11211,7 +11274,7 @@
       <c r="AP176" s="19"/>
       <c r="AQ176" s="19"/>
       <c r="AR176" s="22" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="177" spans="1:44" x14ac:dyDescent="0.25">
@@ -11259,7 +11322,7 @@
       <c r="AP177" s="19"/>
       <c r="AQ177" s="19"/>
       <c r="AR177" s="22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="178" spans="1:44" x14ac:dyDescent="0.25">
@@ -11307,7 +11370,7 @@
       <c r="AP178" s="19"/>
       <c r="AQ178" s="19"/>
       <c r="AR178" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="179" spans="1:44" x14ac:dyDescent="0.25">
@@ -11355,7 +11418,7 @@
       <c r="AP179" s="19"/>
       <c r="AQ179" s="19"/>
       <c r="AR179" s="22" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="180" spans="1:44" x14ac:dyDescent="0.25">
@@ -11403,7 +11466,7 @@
       <c r="AP180" s="19"/>
       <c r="AQ180" s="19"/>
       <c r="AR180" s="22" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="181" spans="1:44" x14ac:dyDescent="0.25">
@@ -11451,7 +11514,7 @@
       <c r="AP181" s="19"/>
       <c r="AQ181" s="19"/>
       <c r="AR181" s="22" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="182" spans="1:44" x14ac:dyDescent="0.25">
@@ -11499,7 +11562,7 @@
       <c r="AP182" s="19"/>
       <c r="AQ182" s="19"/>
       <c r="AR182" s="22" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="183" spans="1:44" x14ac:dyDescent="0.25">
@@ -11547,7 +11610,7 @@
       <c r="AP183" s="19"/>
       <c r="AQ183" s="19"/>
       <c r="AR183" s="22" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="184" spans="1:44" x14ac:dyDescent="0.25">
@@ -11595,7 +11658,7 @@
       <c r="AP184" s="19"/>
       <c r="AQ184" s="19"/>
       <c r="AR184" s="22" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="185" spans="1:44" x14ac:dyDescent="0.25">
@@ -11643,7 +11706,7 @@
       <c r="AP185" s="19"/>
       <c r="AQ185" s="19"/>
       <c r="AR185" s="22" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="186" spans="1:44" x14ac:dyDescent="0.25">
@@ -11691,7 +11754,7 @@
       <c r="AP186" s="19"/>
       <c r="AQ186" s="19"/>
       <c r="AR186" s="22" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="187" spans="1:44" x14ac:dyDescent="0.25">
@@ -11739,7 +11802,7 @@
       <c r="AP187" s="19"/>
       <c r="AQ187" s="19"/>
       <c r="AR187" s="22" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="188" spans="1:44" x14ac:dyDescent="0.25">
@@ -11787,7 +11850,7 @@
       <c r="AP188" s="19"/>
       <c r="AQ188" s="19"/>
       <c r="AR188" s="22" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="189" spans="1:44" x14ac:dyDescent="0.25">
@@ -11835,7 +11898,7 @@
       <c r="AP189" s="19"/>
       <c r="AQ189" s="19"/>
       <c r="AR189" s="22" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="190" spans="1:44" x14ac:dyDescent="0.25">
@@ -11883,7 +11946,7 @@
       <c r="AP190" s="19"/>
       <c r="AQ190" s="19"/>
       <c r="AR190" s="22" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="191" spans="1:44" x14ac:dyDescent="0.25">
@@ -11931,7 +11994,7 @@
       <c r="AP191" s="19"/>
       <c r="AQ191" s="19"/>
       <c r="AR191" s="22" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="192" spans="1:44" x14ac:dyDescent="0.25">
@@ -11979,7 +12042,7 @@
       <c r="AP192" s="19"/>
       <c r="AQ192" s="19"/>
       <c r="AR192" s="22" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="193" spans="1:44" x14ac:dyDescent="0.25">
@@ -12027,7 +12090,7 @@
       <c r="AP193" s="19"/>
       <c r="AQ193" s="19"/>
       <c r="AR193" s="22" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="194" spans="1:44" x14ac:dyDescent="0.25">
@@ -12075,7 +12138,7 @@
       <c r="AP194" s="19"/>
       <c r="AQ194" s="19"/>
       <c r="AR194" s="22" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="195" spans="1:44" x14ac:dyDescent="0.25">
@@ -12123,7 +12186,7 @@
       <c r="AP195" s="19"/>
       <c r="AQ195" s="19"/>
       <c r="AR195" s="22" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="196" spans="1:44" x14ac:dyDescent="0.25">
@@ -12171,7 +12234,7 @@
       <c r="AP196" s="19"/>
       <c r="AQ196" s="19"/>
       <c r="AR196" s="22" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="197" spans="1:44" x14ac:dyDescent="0.25">
@@ -12219,7 +12282,7 @@
       <c r="AP197" s="19"/>
       <c r="AQ197" s="19"/>
       <c r="AR197" s="22" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="198" spans="1:44" x14ac:dyDescent="0.25">
@@ -12267,7 +12330,7 @@
       <c r="AP198" s="19"/>
       <c r="AQ198" s="19"/>
       <c r="AR198" s="22" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="199" spans="1:44" x14ac:dyDescent="0.25">
@@ -12315,7 +12378,7 @@
       <c r="AP199" s="19"/>
       <c r="AQ199" s="19"/>
       <c r="AR199" s="22" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="200" spans="1:44" x14ac:dyDescent="0.25">
@@ -12363,7 +12426,7 @@
       <c r="AP200" s="19"/>
       <c r="AQ200" s="19"/>
       <c r="AR200" s="22" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="201" spans="1:44" x14ac:dyDescent="0.25">
@@ -12411,7 +12474,7 @@
       <c r="AP201" s="19"/>
       <c r="AQ201" s="19"/>
       <c r="AR201" s="22" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="202" spans="1:44" x14ac:dyDescent="0.25">
@@ -12459,7 +12522,7 @@
       <c r="AP202" s="19"/>
       <c r="AQ202" s="19"/>
       <c r="AR202" s="22" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="203" spans="1:44" x14ac:dyDescent="0.25">
@@ -12507,7 +12570,7 @@
       <c r="AP203" s="19"/>
       <c r="AQ203" s="19"/>
       <c r="AR203" s="22" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="204" spans="1:44" x14ac:dyDescent="0.25">
@@ -12555,7 +12618,7 @@
       <c r="AP204" s="19"/>
       <c r="AQ204" s="19"/>
       <c r="AR204" s="22" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="205" spans="1:44" x14ac:dyDescent="0.25">
@@ -12603,7 +12666,7 @@
       <c r="AP205" s="19"/>
       <c r="AQ205" s="19"/>
       <c r="AR205" s="22" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="206" spans="1:44" x14ac:dyDescent="0.25">
@@ -12651,7 +12714,7 @@
       <c r="AP206" s="19"/>
       <c r="AQ206" s="19"/>
       <c r="AR206" s="22" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="207" spans="1:44" x14ac:dyDescent="0.25">
@@ -12699,7 +12762,7 @@
       <c r="AP207" s="19"/>
       <c r="AQ207" s="19"/>
       <c r="AR207" s="22" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="208" spans="1:44" x14ac:dyDescent="0.25">
@@ -12747,7 +12810,7 @@
       <c r="AP208" s="19"/>
       <c r="AQ208" s="19"/>
       <c r="AR208" s="22" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="209" spans="1:44" x14ac:dyDescent="0.25">
@@ -12795,7 +12858,7 @@
       <c r="AP209" s="19"/>
       <c r="AQ209" s="19"/>
       <c r="AR209" s="22" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="210" spans="1:44" x14ac:dyDescent="0.25">
@@ -12843,7 +12906,7 @@
       <c r="AP210" s="19"/>
       <c r="AQ210" s="19"/>
       <c r="AR210" s="22" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="211" spans="1:44" x14ac:dyDescent="0.25">
@@ -12891,7 +12954,7 @@
       <c r="AP211" s="19"/>
       <c r="AQ211" s="19"/>
       <c r="AR211" s="22" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="212" spans="1:44" x14ac:dyDescent="0.25">
@@ -12939,7 +13002,7 @@
       <c r="AP212" s="19"/>
       <c r="AQ212" s="19"/>
       <c r="AR212" s="22" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="213" spans="1:44" x14ac:dyDescent="0.25">
@@ -12987,7 +13050,7 @@
       <c r="AP213" s="19"/>
       <c r="AQ213" s="19"/>
       <c r="AR213" s="22" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="214" spans="1:44" x14ac:dyDescent="0.25">
@@ -13035,7 +13098,7 @@
       <c r="AP214" s="19"/>
       <c r="AQ214" s="19"/>
       <c r="AR214" s="22" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="215" spans="1:44" x14ac:dyDescent="0.25">
@@ -13083,7 +13146,7 @@
       <c r="AP215" s="19"/>
       <c r="AQ215" s="19"/>
       <c r="AR215" s="22" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="216" spans="1:44" x14ac:dyDescent="0.25">
@@ -13131,7 +13194,7 @@
       <c r="AP216" s="19"/>
       <c r="AQ216" s="19"/>
       <c r="AR216" s="22" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="217" spans="1:44" x14ac:dyDescent="0.25">
@@ -13179,7 +13242,7 @@
       <c r="AP217" s="19"/>
       <c r="AQ217" s="19"/>
       <c r="AR217" s="22" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="218" spans="1:44" x14ac:dyDescent="0.25">
@@ -13227,7 +13290,7 @@
       <c r="AP218" s="19"/>
       <c r="AQ218" s="19"/>
       <c r="AR218" s="22" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="219" spans="1:44" x14ac:dyDescent="0.25">
@@ -13275,7 +13338,7 @@
       <c r="AP219" s="19"/>
       <c r="AQ219" s="19"/>
       <c r="AR219" s="22" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="220" spans="1:44" x14ac:dyDescent="0.25">
@@ -13323,7 +13386,7 @@
       <c r="AP220" s="19"/>
       <c r="AQ220" s="19"/>
       <c r="AR220" s="22" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="221" spans="1:44" x14ac:dyDescent="0.25">
@@ -13371,7 +13434,7 @@
       <c r="AP221" s="19"/>
       <c r="AQ221" s="19"/>
       <c r="AR221" s="22" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="222" spans="1:44" x14ac:dyDescent="0.25">
@@ -13419,7 +13482,7 @@
       <c r="AP222" s="19"/>
       <c r="AQ222" s="19"/>
       <c r="AR222" s="22" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="223" spans="1:44" x14ac:dyDescent="0.25">
@@ -13467,7 +13530,7 @@
       <c r="AP223" s="19"/>
       <c r="AQ223" s="19"/>
       <c r="AR223" s="22" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="224" spans="1:44" x14ac:dyDescent="0.25">
@@ -13515,7 +13578,7 @@
       <c r="AP224" s="19"/>
       <c r="AQ224" s="19"/>
       <c r="AR224" s="22" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="225" spans="1:44" x14ac:dyDescent="0.25">
@@ -13563,7 +13626,7 @@
       <c r="AP225" s="19"/>
       <c r="AQ225" s="19"/>
       <c r="AR225" s="22" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="226" spans="1:44" x14ac:dyDescent="0.25">
@@ -13611,7 +13674,7 @@
       <c r="AP226" s="19"/>
       <c r="AQ226" s="19"/>
       <c r="AR226" s="22" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="227" spans="1:44" x14ac:dyDescent="0.25">
@@ -13659,7 +13722,7 @@
       <c r="AP227" s="19"/>
       <c r="AQ227" s="19"/>
       <c r="AR227" s="22" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="228" spans="1:44" x14ac:dyDescent="0.25">
@@ -13707,7 +13770,7 @@
       <c r="AP228" s="19"/>
       <c r="AQ228" s="19"/>
       <c r="AR228" s="22" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="229" spans="1:44" x14ac:dyDescent="0.25">
@@ -13755,7 +13818,7 @@
       <c r="AP229" s="19"/>
       <c r="AQ229" s="19"/>
       <c r="AR229" s="22" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="230" spans="1:44" x14ac:dyDescent="0.25">
@@ -13803,7 +13866,7 @@
       <c r="AP230" s="19"/>
       <c r="AQ230" s="19"/>
       <c r="AR230" s="22" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="231" spans="1:44" x14ac:dyDescent="0.25">
@@ -13851,7 +13914,7 @@
       <c r="AP231" s="19"/>
       <c r="AQ231" s="19"/>
       <c r="AR231" s="22" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="232" spans="1:44" x14ac:dyDescent="0.25">
@@ -13899,7 +13962,7 @@
       <c r="AP232" s="19"/>
       <c r="AQ232" s="19"/>
       <c r="AR232" s="22" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="233" spans="1:44" x14ac:dyDescent="0.25">
@@ -13947,7 +14010,7 @@
       <c r="AP233" s="19"/>
       <c r="AQ233" s="19"/>
       <c r="AR233" s="22" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="234" spans="1:44" x14ac:dyDescent="0.25">
@@ -13995,7 +14058,7 @@
       <c r="AP234" s="19"/>
       <c r="AQ234" s="19"/>
       <c r="AR234" s="22" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="235" spans="1:44" x14ac:dyDescent="0.25">
@@ -14043,7 +14106,7 @@
       <c r="AP235" s="19"/>
       <c r="AQ235" s="19"/>
       <c r="AR235" s="22" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="236" spans="1:44" x14ac:dyDescent="0.25">
@@ -14091,7 +14154,7 @@
       <c r="AP236" s="19"/>
       <c r="AQ236" s="19"/>
       <c r="AR236" s="22" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="237" spans="1:44" x14ac:dyDescent="0.25">
@@ -14139,7 +14202,7 @@
       <c r="AP237" s="19"/>
       <c r="AQ237" s="19"/>
       <c r="AR237" s="22" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="238" spans="1:44" x14ac:dyDescent="0.25">
@@ -14187,7 +14250,7 @@
       <c r="AP238" s="19"/>
       <c r="AQ238" s="19"/>
       <c r="AR238" s="22" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="239" spans="1:44" x14ac:dyDescent="0.25">
@@ -14235,7 +14298,7 @@
       <c r="AP239" s="19"/>
       <c r="AQ239" s="19"/>
       <c r="AR239" s="22" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="240" spans="1:44" x14ac:dyDescent="0.25">
@@ -14283,7 +14346,7 @@
       <c r="AP240" s="19"/>
       <c r="AQ240" s="19"/>
       <c r="AR240" s="22" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="241" spans="1:44" x14ac:dyDescent="0.25">
@@ -14331,7 +14394,7 @@
       <c r="AP241" s="19"/>
       <c r="AQ241" s="19"/>
       <c r="AR241" s="22" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="242" spans="1:44" x14ac:dyDescent="0.25">
@@ -14379,7 +14442,7 @@
       <c r="AP242" s="19"/>
       <c r="AQ242" s="19"/>
       <c r="AR242" s="22" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="243" spans="1:44" x14ac:dyDescent="0.25">
@@ -14427,7 +14490,7 @@
       <c r="AP243" s="19"/>
       <c r="AQ243" s="19"/>
       <c r="AR243" s="22" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="244" spans="1:44" x14ac:dyDescent="0.25">
@@ -14475,7 +14538,7 @@
       <c r="AP244" s="19"/>
       <c r="AQ244" s="19"/>
       <c r="AR244" s="22" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="245" spans="1:44" x14ac:dyDescent="0.25">
@@ -14523,7 +14586,7 @@
       <c r="AP245" s="19"/>
       <c r="AQ245" s="19"/>
       <c r="AR245" s="22" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="246" spans="1:44" x14ac:dyDescent="0.25">
@@ -14571,7 +14634,7 @@
       <c r="AP246" s="19"/>
       <c r="AQ246" s="19"/>
       <c r="AR246" s="22" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="247" spans="1:44" x14ac:dyDescent="0.25">
@@ -14619,7 +14682,7 @@
       <c r="AP247" s="19"/>
       <c r="AQ247" s="19"/>
       <c r="AR247" s="22" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="248" spans="1:44" x14ac:dyDescent="0.25">
@@ -14667,7 +14730,7 @@
       <c r="AP248" s="19"/>
       <c r="AQ248" s="19"/>
       <c r="AR248" s="22" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="249" spans="1:44" x14ac:dyDescent="0.25">
@@ -14715,7 +14778,7 @@
       <c r="AP249" s="19"/>
       <c r="AQ249" s="19"/>
       <c r="AR249" s="22" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="250" spans="1:44" x14ac:dyDescent="0.25">
@@ -14763,7 +14826,7 @@
       <c r="AP250" s="19"/>
       <c r="AQ250" s="19"/>
       <c r="AR250" s="22" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="251" spans="1:44" x14ac:dyDescent="0.25">
@@ -14811,7 +14874,7 @@
       <c r="AP251" s="19"/>
       <c r="AQ251" s="19"/>
       <c r="AR251" s="22" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="252" spans="1:44" x14ac:dyDescent="0.25">
@@ -14859,7 +14922,7 @@
       <c r="AP252" s="19"/>
       <c r="AQ252" s="19"/>
       <c r="AR252" s="22" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="253" spans="1:44" x14ac:dyDescent="0.25">
@@ -14907,7 +14970,7 @@
       <c r="AP253" s="19"/>
       <c r="AQ253" s="19"/>
       <c r="AR253" s="22" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="254" spans="1:44" x14ac:dyDescent="0.25">
@@ -14955,7 +15018,7 @@
       <c r="AP254" s="19"/>
       <c r="AQ254" s="19"/>
       <c r="AR254" s="22" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="255" spans="1:44" x14ac:dyDescent="0.25">
@@ -15003,7 +15066,7 @@
       <c r="AP255" s="19"/>
       <c r="AQ255" s="19"/>
       <c r="AR255" s="22" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="256" spans="1:44" x14ac:dyDescent="0.25">
@@ -15051,7 +15114,7 @@
       <c r="AP256" s="19"/>
       <c r="AQ256" s="19"/>
       <c r="AR256" s="22" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="257" spans="1:44" x14ac:dyDescent="0.25">
@@ -15099,7 +15162,7 @@
       <c r="AP257" s="19"/>
       <c r="AQ257" s="19"/>
       <c r="AR257" s="22" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="258" spans="1:44" x14ac:dyDescent="0.25">
@@ -15147,7 +15210,7 @@
       <c r="AP258" s="19"/>
       <c r="AQ258" s="19"/>
       <c r="AR258" s="22" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="259" spans="1:44" x14ac:dyDescent="0.25">
@@ -15195,7 +15258,7 @@
       <c r="AP259" s="19"/>
       <c r="AQ259" s="19"/>
       <c r="AR259" s="22" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="260" spans="1:44" x14ac:dyDescent="0.25">
@@ -15243,7 +15306,7 @@
       <c r="AP260" s="19"/>
       <c r="AQ260" s="19"/>
       <c r="AR260" s="22" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="261" spans="1:44" x14ac:dyDescent="0.25">
@@ -15291,7 +15354,7 @@
       <c r="AP261" s="19"/>
       <c r="AQ261" s="19"/>
       <c r="AR261" s="22" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="262" spans="1:44" x14ac:dyDescent="0.25">
@@ -15339,7 +15402,7 @@
       <c r="AP262" s="19"/>
       <c r="AQ262" s="19"/>
       <c r="AR262" s="22" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="263" spans="1:44" x14ac:dyDescent="0.25">
@@ -15387,7 +15450,7 @@
       <c r="AP263" s="19"/>
       <c r="AQ263" s="19"/>
       <c r="AR263" s="22" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="264" spans="1:44" x14ac:dyDescent="0.25">
@@ -15435,7 +15498,7 @@
       <c r="AP264" s="19"/>
       <c r="AQ264" s="19"/>
       <c r="AR264" s="22" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="265" spans="1:44" x14ac:dyDescent="0.25">
@@ -15483,7 +15546,7 @@
       <c r="AP265" s="19"/>
       <c r="AQ265" s="19"/>
       <c r="AR265" s="22" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="266" spans="1:44" x14ac:dyDescent="0.25">
@@ -15531,7 +15594,7 @@
       <c r="AP266" s="19"/>
       <c r="AQ266" s="19"/>
       <c r="AR266" s="22" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="267" spans="1:44" x14ac:dyDescent="0.25">
@@ -15579,7 +15642,7 @@
       <c r="AP267" s="19"/>
       <c r="AQ267" s="19"/>
       <c r="AR267" s="22" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="268" spans="1:44" x14ac:dyDescent="0.25">
@@ -15627,7 +15690,7 @@
       <c r="AP268" s="19"/>
       <c r="AQ268" s="19"/>
       <c r="AR268" s="22" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="269" spans="1:44" x14ac:dyDescent="0.25">
@@ -15675,7 +15738,7 @@
       <c r="AP269" s="19"/>
       <c r="AQ269" s="19"/>
       <c r="AR269" s="22" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="270" spans="1:44" x14ac:dyDescent="0.25">
@@ -15723,7 +15786,7 @@
       <c r="AP270" s="19"/>
       <c r="AQ270" s="19"/>
       <c r="AR270" s="22" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="271" spans="1:44" x14ac:dyDescent="0.25">
@@ -15771,7 +15834,7 @@
       <c r="AP271" s="19"/>
       <c r="AQ271" s="19"/>
       <c r="AR271" s="22" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="272" spans="1:44" x14ac:dyDescent="0.25">
@@ -15819,7 +15882,7 @@
       <c r="AP272" s="19"/>
       <c r="AQ272" s="19"/>
       <c r="AR272" s="22" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="273" spans="1:44" x14ac:dyDescent="0.25">
@@ -15867,7 +15930,7 @@
       <c r="AP273" s="19"/>
       <c r="AQ273" s="19"/>
       <c r="AR273" s="22" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="274" spans="1:44" x14ac:dyDescent="0.25">
@@ -15915,7 +15978,7 @@
       <c r="AP274" s="19"/>
       <c r="AQ274" s="19"/>
       <c r="AR274" s="22" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="275" spans="1:44" x14ac:dyDescent="0.25">
@@ -15963,7 +16026,7 @@
       <c r="AP275" s="19"/>
       <c r="AQ275" s="19"/>
       <c r="AR275" s="22" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="276" spans="1:44" x14ac:dyDescent="0.25">
@@ -16011,7 +16074,7 @@
       <c r="AP276" s="19"/>
       <c r="AQ276" s="19"/>
       <c r="AR276" s="22" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="277" spans="1:44" x14ac:dyDescent="0.25">
@@ -16059,7 +16122,7 @@
       <c r="AP277" s="19"/>
       <c r="AQ277" s="19"/>
       <c r="AR277" s="22" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="278" spans="1:44" x14ac:dyDescent="0.25">
@@ -16107,7 +16170,7 @@
       <c r="AP278" s="19"/>
       <c r="AQ278" s="19"/>
       <c r="AR278" s="22" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="279" spans="1:44" x14ac:dyDescent="0.25">
@@ -16155,7 +16218,7 @@
       <c r="AP279" s="19"/>
       <c r="AQ279" s="19"/>
       <c r="AR279" s="22" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="280" spans="1:44" x14ac:dyDescent="0.25">
@@ -16203,7 +16266,7 @@
       <c r="AP280" s="19"/>
       <c r="AQ280" s="19"/>
       <c r="AR280" s="22" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="281" spans="1:44" x14ac:dyDescent="0.25">
@@ -16251,7 +16314,7 @@
       <c r="AP281" s="19"/>
       <c r="AQ281" s="19"/>
       <c r="AR281" s="22" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="282" spans="1:44" x14ac:dyDescent="0.25">
@@ -16299,7 +16362,7 @@
       <c r="AP282" s="19"/>
       <c r="AQ282" s="19"/>
       <c r="AR282" s="22" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="283" spans="1:44" x14ac:dyDescent="0.25">
@@ -16347,7 +16410,7 @@
       <c r="AP283" s="19"/>
       <c r="AQ283" s="19"/>
       <c r="AR283" s="22" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="284" spans="1:44" x14ac:dyDescent="0.25">
@@ -16395,7 +16458,7 @@
       <c r="AP284" s="19"/>
       <c r="AQ284" s="19"/>
       <c r="AR284" s="22" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="285" spans="1:44" x14ac:dyDescent="0.25">
@@ -16443,7 +16506,7 @@
       <c r="AP285" s="19"/>
       <c r="AQ285" s="19"/>
       <c r="AR285" s="22" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="286" spans="1:44" x14ac:dyDescent="0.25">
@@ -16491,7 +16554,7 @@
       <c r="AP286" s="19"/>
       <c r="AQ286" s="19"/>
       <c r="AR286" s="22" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="287" spans="1:44" x14ac:dyDescent="0.25">
@@ -16539,7 +16602,7 @@
       <c r="AP287" s="19"/>
       <c r="AQ287" s="19"/>
       <c r="AR287" s="22" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="288" spans="1:44" x14ac:dyDescent="0.25">
@@ -16587,7 +16650,7 @@
       <c r="AP288" s="19"/>
       <c r="AQ288" s="19"/>
       <c r="AR288" s="22" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="289" spans="1:44" x14ac:dyDescent="0.25">
@@ -16635,7 +16698,7 @@
       <c r="AP289" s="19"/>
       <c r="AQ289" s="19"/>
       <c r="AR289" s="22" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="290" spans="1:44" x14ac:dyDescent="0.25">
@@ -16683,7 +16746,7 @@
       <c r="AP290" s="19"/>
       <c r="AQ290" s="19"/>
       <c r="AR290" s="22" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="291" spans="1:44" x14ac:dyDescent="0.25">
@@ -16731,7 +16794,7 @@
       <c r="AP291" s="19"/>
       <c r="AQ291" s="19"/>
       <c r="AR291" s="22" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="292" spans="1:44" x14ac:dyDescent="0.25">
@@ -16779,7 +16842,7 @@
       <c r="AP292" s="19"/>
       <c r="AQ292" s="19"/>
       <c r="AR292" s="22" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="293" spans="1:44" x14ac:dyDescent="0.25">
@@ -16827,7 +16890,7 @@
       <c r="AP293" s="19"/>
       <c r="AQ293" s="19"/>
       <c r="AR293" s="22" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="294" spans="1:44" x14ac:dyDescent="0.25">
@@ -16875,7 +16938,7 @@
       <c r="AP294" s="19"/>
       <c r="AQ294" s="19"/>
       <c r="AR294" s="22" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="295" spans="1:44" x14ac:dyDescent="0.25">
@@ -16923,7 +16986,7 @@
       <c r="AP295" s="19"/>
       <c r="AQ295" s="19"/>
       <c r="AR295" s="22" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="296" spans="1:44" x14ac:dyDescent="0.25">
@@ -16971,7 +17034,7 @@
       <c r="AP296" s="19"/>
       <c r="AQ296" s="19"/>
       <c r="AR296" s="22" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="297" spans="1:44" x14ac:dyDescent="0.25">
@@ -17019,7 +17082,7 @@
       <c r="AP297" s="19"/>
       <c r="AQ297" s="19"/>
       <c r="AR297" s="22" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="298" spans="1:44" x14ac:dyDescent="0.25">
@@ -17067,7 +17130,7 @@
       <c r="AP298" s="19"/>
       <c r="AQ298" s="19"/>
       <c r="AR298" s="22" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="299" spans="1:44" x14ac:dyDescent="0.25">
@@ -17115,7 +17178,7 @@
       <c r="AP299" s="19"/>
       <c r="AQ299" s="19"/>
       <c r="AR299" s="22" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="300" spans="1:44" x14ac:dyDescent="0.25">
@@ -17163,7 +17226,7 @@
       <c r="AP300" s="19"/>
       <c r="AQ300" s="19"/>
       <c r="AR300" s="22" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="301" spans="1:44" x14ac:dyDescent="0.25">
@@ -17211,7 +17274,7 @@
       <c r="AP301" s="19"/>
       <c r="AQ301" s="19"/>
       <c r="AR301" s="22" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="302" spans="1:44" x14ac:dyDescent="0.25">
@@ -17259,7 +17322,7 @@
       <c r="AP302" s="19"/>
       <c r="AQ302" s="19"/>
       <c r="AR302" s="22" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="303" spans="1:44" x14ac:dyDescent="0.25">
@@ -17307,7 +17370,7 @@
       <c r="AP303" s="19"/>
       <c r="AQ303" s="19"/>
       <c r="AR303" s="22" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="304" spans="1:44" x14ac:dyDescent="0.25">
@@ -17355,7 +17418,7 @@
       <c r="AP304" s="19"/>
       <c r="AQ304" s="19"/>
       <c r="AR304" s="22" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="305" spans="1:44" x14ac:dyDescent="0.25">
@@ -17403,7 +17466,7 @@
       <c r="AP305" s="19"/>
       <c r="AQ305" s="19"/>
       <c r="AR305" s="22" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="306" spans="1:44" x14ac:dyDescent="0.25">
@@ -17451,7 +17514,7 @@
       <c r="AP306" s="19"/>
       <c r="AQ306" s="19"/>
       <c r="AR306" s="22" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="307" spans="1:44" x14ac:dyDescent="0.25">
@@ -17499,7 +17562,7 @@
       <c r="AP307" s="19"/>
       <c r="AQ307" s="19"/>
       <c r="AR307" s="22" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="308" spans="1:44" x14ac:dyDescent="0.25">
@@ -17547,7 +17610,7 @@
       <c r="AP308" s="19"/>
       <c r="AQ308" s="19"/>
       <c r="AR308" s="22" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="309" spans="1:44" x14ac:dyDescent="0.25">
@@ -17595,7 +17658,7 @@
       <c r="AP309" s="19"/>
       <c r="AQ309" s="19"/>
       <c r="AR309" s="22" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="310" spans="1:44" x14ac:dyDescent="0.25">
@@ -17643,7 +17706,7 @@
       <c r="AP310" s="19"/>
       <c r="AQ310" s="19"/>
       <c r="AR310" s="22" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="311" spans="1:44" x14ac:dyDescent="0.25">
@@ -17691,7 +17754,7 @@
       <c r="AP311" s="19"/>
       <c r="AQ311" s="19"/>
       <c r="AR311" s="22" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="312" spans="1:44" x14ac:dyDescent="0.25">
@@ -17739,7 +17802,7 @@
       <c r="AP312" s="19"/>
       <c r="AQ312" s="19"/>
       <c r="AR312" s="22" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="313" spans="1:44" x14ac:dyDescent="0.25">
@@ -17787,7 +17850,7 @@
       <c r="AP313" s="19"/>
       <c r="AQ313" s="19"/>
       <c r="AR313" s="22" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="314" spans="1:44" x14ac:dyDescent="0.25">
@@ -17835,7 +17898,7 @@
       <c r="AP314" s="19"/>
       <c r="AQ314" s="19"/>
       <c r="AR314" s="22" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="315" spans="1:44" x14ac:dyDescent="0.25">
@@ -17883,7 +17946,7 @@
       <c r="AP315" s="19"/>
       <c r="AQ315" s="19"/>
       <c r="AR315" s="22" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="316" spans="1:44" x14ac:dyDescent="0.25">
@@ -17931,7 +17994,7 @@
       <c r="AP316" s="19"/>
       <c r="AQ316" s="19"/>
       <c r="AR316" s="22" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="317" spans="1:44" x14ac:dyDescent="0.25">
@@ -17979,7 +18042,7 @@
       <c r="AP317" s="19"/>
       <c r="AQ317" s="19"/>
       <c r="AR317" s="22" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="318" spans="1:44" x14ac:dyDescent="0.25">
@@ -18027,7 +18090,7 @@
       <c r="AP318" s="19"/>
       <c r="AQ318" s="19"/>
       <c r="AR318" s="22" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="319" spans="1:44" x14ac:dyDescent="0.25">
@@ -18075,7 +18138,7 @@
       <c r="AP319" s="19"/>
       <c r="AQ319" s="19"/>
       <c r="AR319" s="22" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="320" spans="1:44" x14ac:dyDescent="0.25">
@@ -18123,7 +18186,7 @@
       <c r="AP320" s="19"/>
       <c r="AQ320" s="19"/>
       <c r="AR320" s="22" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="321" spans="1:44" x14ac:dyDescent="0.25">
@@ -18171,7 +18234,7 @@
       <c r="AP321" s="19"/>
       <c r="AQ321" s="19"/>
       <c r="AR321" s="22" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="322" spans="1:44" x14ac:dyDescent="0.25">
@@ -18219,7 +18282,7 @@
       <c r="AP322" s="19"/>
       <c r="AQ322" s="19"/>
       <c r="AR322" s="22" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="323" spans="1:44" x14ac:dyDescent="0.25">
@@ -18267,7 +18330,7 @@
       <c r="AP323" s="19"/>
       <c r="AQ323" s="19"/>
       <c r="AR323" s="22" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="324" spans="1:44" x14ac:dyDescent="0.25">
@@ -18315,7 +18378,7 @@
       <c r="AP324" s="19"/>
       <c r="AQ324" s="19"/>
       <c r="AR324" s="22" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="325" spans="1:44" x14ac:dyDescent="0.25">
@@ -18363,7 +18426,7 @@
       <c r="AP325" s="19"/>
       <c r="AQ325" s="19"/>
       <c r="AR325" s="22" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="326" spans="1:44" x14ac:dyDescent="0.25">
@@ -18411,7 +18474,7 @@
       <c r="AP326" s="19"/>
       <c r="AQ326" s="19"/>
       <c r="AR326" s="22" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="327" spans="1:44" x14ac:dyDescent="0.25">
@@ -18459,7 +18522,7 @@
       <c r="AP327" s="19"/>
       <c r="AQ327" s="19"/>
       <c r="AR327" s="22" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="328" spans="1:44" x14ac:dyDescent="0.25">
@@ -18507,7 +18570,7 @@
       <c r="AP328" s="19"/>
       <c r="AQ328" s="19"/>
       <c r="AR328" s="22" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="329" spans="1:44" x14ac:dyDescent="0.25">
@@ -18555,7 +18618,7 @@
       <c r="AP329" s="19"/>
       <c r="AQ329" s="19"/>
       <c r="AR329" s="22" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="330" spans="1:44" x14ac:dyDescent="0.25">
@@ -18603,7 +18666,7 @@
       <c r="AP330" s="19"/>
       <c r="AQ330" s="19"/>
       <c r="AR330" s="22" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="331" spans="1:44" x14ac:dyDescent="0.25">
@@ -18651,7 +18714,7 @@
       <c r="AP331" s="19"/>
       <c r="AQ331" s="19"/>
       <c r="AR331" s="22" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="332" spans="1:44" x14ac:dyDescent="0.25">
@@ -18699,7 +18762,7 @@
       <c r="AP332" s="19"/>
       <c r="AQ332" s="19"/>
       <c r="AR332" s="22" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="333" spans="1:44" x14ac:dyDescent="0.25">
@@ -18747,7 +18810,7 @@
       <c r="AP333" s="19"/>
       <c r="AQ333" s="19"/>
       <c r="AR333" s="22" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="334" spans="1:44" x14ac:dyDescent="0.25">
@@ -18795,7 +18858,7 @@
       <c r="AP334" s="19"/>
       <c r="AQ334" s="19"/>
       <c r="AR334" s="22" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="335" spans="1:44" x14ac:dyDescent="0.25">
@@ -18843,7 +18906,7 @@
       <c r="AP335" s="19"/>
       <c r="AQ335" s="19"/>
       <c r="AR335" s="22" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="336" spans="1:44" x14ac:dyDescent="0.25">
@@ -18891,7 +18954,7 @@
       <c r="AP336" s="19"/>
       <c r="AQ336" s="19"/>
       <c r="AR336" s="22" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="337" spans="1:44" x14ac:dyDescent="0.25">
@@ -18939,7 +19002,7 @@
       <c r="AP337" s="19"/>
       <c r="AQ337" s="19"/>
       <c r="AR337" s="22" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="338" spans="1:44" x14ac:dyDescent="0.25">
@@ -18987,7 +19050,7 @@
       <c r="AP338" s="19"/>
       <c r="AQ338" s="19"/>
       <c r="AR338" s="22" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="339" spans="1:44" x14ac:dyDescent="0.25">
@@ -19035,7 +19098,7 @@
       <c r="AP339" s="19"/>
       <c r="AQ339" s="19"/>
       <c r="AR339" s="22" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="340" spans="1:44" x14ac:dyDescent="0.25">
@@ -19083,7 +19146,7 @@
       <c r="AP340" s="19"/>
       <c r="AQ340" s="19"/>
       <c r="AR340" s="22" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="341" spans="1:44" x14ac:dyDescent="0.25">
@@ -19131,7 +19194,7 @@
       <c r="AP341" s="19"/>
       <c r="AQ341" s="19"/>
       <c r="AR341" s="22" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="342" spans="1:44" x14ac:dyDescent="0.25">
@@ -19179,7 +19242,7 @@
       <c r="AP342" s="19"/>
       <c r="AQ342" s="19"/>
       <c r="AR342" s="22" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="343" spans="1:44" x14ac:dyDescent="0.25">
@@ -19227,7 +19290,7 @@
       <c r="AP343" s="19"/>
       <c r="AQ343" s="19"/>
       <c r="AR343" s="22" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="344" spans="1:44" x14ac:dyDescent="0.25">
@@ -19275,7 +19338,7 @@
       <c r="AP344" s="19"/>
       <c r="AQ344" s="19"/>
       <c r="AR344" s="22" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="345" spans="1:44" x14ac:dyDescent="0.25">
@@ -19323,7 +19386,7 @@
       <c r="AP345" s="19"/>
       <c r="AQ345" s="19"/>
       <c r="AR345" s="22" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="346" spans="1:44" x14ac:dyDescent="0.25">
@@ -19371,7 +19434,7 @@
       <c r="AP346" s="19"/>
       <c r="AQ346" s="19"/>
       <c r="AR346" s="22" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="347" spans="1:44" x14ac:dyDescent="0.25">
@@ -19419,7 +19482,7 @@
       <c r="AP347" s="19"/>
       <c r="AQ347" s="19"/>
       <c r="AR347" s="22" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="348" spans="1:44" x14ac:dyDescent="0.25">
@@ -19467,7 +19530,7 @@
       <c r="AP348" s="19"/>
       <c r="AQ348" s="19"/>
       <c r="AR348" s="22" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="349" spans="1:44" x14ac:dyDescent="0.25">
@@ -19515,7 +19578,7 @@
       <c r="AP349" s="19"/>
       <c r="AQ349" s="19"/>
       <c r="AR349" s="22" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="350" spans="1:44" x14ac:dyDescent="0.25">
@@ -19563,7 +19626,7 @@
       <c r="AP350" s="19"/>
       <c r="AQ350" s="19"/>
       <c r="AR350" s="22" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="351" spans="1:44" x14ac:dyDescent="0.25">
@@ -19611,7 +19674,7 @@
       <c r="AP351" s="19"/>
       <c r="AQ351" s="19"/>
       <c r="AR351" s="22" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="352" spans="1:44" x14ac:dyDescent="0.25">
@@ -19659,7 +19722,7 @@
       <c r="AP352" s="19"/>
       <c r="AQ352" s="19"/>
       <c r="AR352" s="22" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="353" spans="1:44" x14ac:dyDescent="0.25">
@@ -19707,7 +19770,7 @@
       <c r="AP353" s="19"/>
       <c r="AQ353" s="19"/>
       <c r="AR353" s="22" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="354" spans="1:44" x14ac:dyDescent="0.25">
@@ -19755,7 +19818,7 @@
       <c r="AP354" s="19"/>
       <c r="AQ354" s="19"/>
       <c r="AR354" s="22" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="355" spans="1:44" x14ac:dyDescent="0.25">
@@ -19803,7 +19866,7 @@
       <c r="AP355" s="19"/>
       <c r="AQ355" s="19"/>
       <c r="AR355" s="22" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="356" spans="1:44" x14ac:dyDescent="0.25">
@@ -19851,7 +19914,7 @@
       <c r="AP356" s="19"/>
       <c r="AQ356" s="19"/>
       <c r="AR356" s="22" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="357" spans="1:44" x14ac:dyDescent="0.25">
@@ -19899,7 +19962,7 @@
       <c r="AP357" s="19"/>
       <c r="AQ357" s="19"/>
       <c r="AR357" s="22" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="358" spans="1:44" x14ac:dyDescent="0.25">
@@ -19947,7 +20010,7 @@
       <c r="AP358" s="19"/>
       <c r="AQ358" s="19"/>
       <c r="AR358" s="22" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="359" spans="1:44" x14ac:dyDescent="0.25">
@@ -19995,7 +20058,7 @@
       <c r="AP359" s="19"/>
       <c r="AQ359" s="19"/>
       <c r="AR359" s="22" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="360" spans="1:44" x14ac:dyDescent="0.25">
@@ -20043,7 +20106,7 @@
       <c r="AP360" s="19"/>
       <c r="AQ360" s="19"/>
       <c r="AR360" s="22" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="361" spans="1:44" x14ac:dyDescent="0.25">
@@ -20091,7 +20154,7 @@
       <c r="AP361" s="19"/>
       <c r="AQ361" s="19"/>
       <c r="AR361" s="22" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="362" spans="1:44" x14ac:dyDescent="0.25">
@@ -20139,7 +20202,7 @@
       <c r="AP362" s="19"/>
       <c r="AQ362" s="19"/>
       <c r="AR362" s="22" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="363" spans="1:44" x14ac:dyDescent="0.25">
@@ -20187,7 +20250,7 @@
       <c r="AP363" s="19"/>
       <c r="AQ363" s="19"/>
       <c r="AR363" s="22" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="364" spans="1:44" x14ac:dyDescent="0.25">
@@ -20235,7 +20298,7 @@
       <c r="AP364" s="19"/>
       <c r="AQ364" s="19"/>
       <c r="AR364" s="22" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="365" spans="1:44" x14ac:dyDescent="0.25">
@@ -20283,7 +20346,7 @@
       <c r="AP365" s="19"/>
       <c r="AQ365" s="19"/>
       <c r="AR365" s="22" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="366" spans="1:44" x14ac:dyDescent="0.25">
@@ -20331,7 +20394,7 @@
       <c r="AP366" s="19"/>
       <c r="AQ366" s="19"/>
       <c r="AR366" s="22" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="367" spans="1:44" x14ac:dyDescent="0.25">
@@ -20379,7 +20442,7 @@
       <c r="AP367" s="19"/>
       <c r="AQ367" s="19"/>
       <c r="AR367" s="22" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="368" spans="1:44" x14ac:dyDescent="0.25">
@@ -20427,7 +20490,7 @@
       <c r="AP368" s="19"/>
       <c r="AQ368" s="19"/>
       <c r="AR368" s="22" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="369" spans="1:44" x14ac:dyDescent="0.25">
@@ -20475,7 +20538,7 @@
       <c r="AP369" s="19"/>
       <c r="AQ369" s="19"/>
       <c r="AR369" s="22" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="370" spans="1:44" x14ac:dyDescent="0.25">
@@ -20523,7 +20586,7 @@
       <c r="AP370" s="19"/>
       <c r="AQ370" s="19"/>
       <c r="AR370" s="22" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="371" spans="1:44" x14ac:dyDescent="0.25">
@@ -20571,7 +20634,7 @@
       <c r="AP371" s="19"/>
       <c r="AQ371" s="19"/>
       <c r="AR371" s="22" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="372" spans="1:44" x14ac:dyDescent="0.25">
@@ -20619,7 +20682,7 @@
       <c r="AP372" s="19"/>
       <c r="AQ372" s="19"/>
       <c r="AR372" s="22" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="373" spans="1:44" x14ac:dyDescent="0.25">
@@ -20667,7 +20730,7 @@
       <c r="AP373" s="19"/>
       <c r="AQ373" s="19"/>
       <c r="AR373" s="22" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="374" spans="1:44" x14ac:dyDescent="0.25">
@@ -20715,7 +20778,7 @@
       <c r="AP374" s="19"/>
       <c r="AQ374" s="19"/>
       <c r="AR374" s="22" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="375" spans="1:44" x14ac:dyDescent="0.25">
@@ -20763,7 +20826,7 @@
       <c r="AP375" s="19"/>
       <c r="AQ375" s="19"/>
       <c r="AR375" s="22" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="376" spans="1:44" x14ac:dyDescent="0.25">
@@ -20811,7 +20874,7 @@
       <c r="AP376" s="19"/>
       <c r="AQ376" s="19"/>
       <c r="AR376" s="22" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="377" spans="1:44" x14ac:dyDescent="0.25">
@@ -20859,7 +20922,7 @@
       <c r="AP377" s="19"/>
       <c r="AQ377" s="19"/>
       <c r="AR377" s="22" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="378" spans="1:44" x14ac:dyDescent="0.25">
@@ -20907,7 +20970,7 @@
       <c r="AP378" s="19"/>
       <c r="AQ378" s="19"/>
       <c r="AR378" s="22" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="379" spans="1:44" x14ac:dyDescent="0.25">
@@ -20955,7 +21018,7 @@
       <c r="AP379" s="19"/>
       <c r="AQ379" s="19"/>
       <c r="AR379" s="22" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="380" spans="1:44" x14ac:dyDescent="0.25">
@@ -21003,7 +21066,7 @@
       <c r="AP380" s="19"/>
       <c r="AQ380" s="19"/>
       <c r="AR380" s="22" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="381" spans="1:44" x14ac:dyDescent="0.25">
@@ -21051,7 +21114,7 @@
       <c r="AP381" s="19"/>
       <c r="AQ381" s="19"/>
       <c r="AR381" s="22" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="382" spans="1:44" x14ac:dyDescent="0.25">
@@ -21099,7 +21162,7 @@
       <c r="AP382" s="19"/>
       <c r="AQ382" s="19"/>
       <c r="AR382" s="22" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="383" spans="1:44" x14ac:dyDescent="0.25">
@@ -21147,7 +21210,7 @@
       <c r="AP383" s="19"/>
       <c r="AQ383" s="19"/>
       <c r="AR383" s="22" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="384" spans="1:44" x14ac:dyDescent="0.25">
@@ -21195,7 +21258,7 @@
       <c r="AP384" s="19"/>
       <c r="AQ384" s="19"/>
       <c r="AR384" s="22" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="385" spans="1:44" x14ac:dyDescent="0.25">
@@ -21243,7 +21306,7 @@
       <c r="AP385" s="19"/>
       <c r="AQ385" s="19"/>
       <c r="AR385" s="22" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="386" spans="1:44" x14ac:dyDescent="0.25">
@@ -21291,7 +21354,7 @@
       <c r="AP386" s="19"/>
       <c r="AQ386" s="19"/>
       <c r="AR386" s="22" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="387" spans="1:44" x14ac:dyDescent="0.25">
@@ -21339,7 +21402,7 @@
       <c r="AP387" s="19"/>
       <c r="AQ387" s="19"/>
       <c r="AR387" s="22" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="388" spans="1:44" x14ac:dyDescent="0.25">
@@ -21387,7 +21450,7 @@
       <c r="AP388" s="19"/>
       <c r="AQ388" s="19"/>
       <c r="AR388" s="22" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="389" spans="1:44" x14ac:dyDescent="0.25">
@@ -21435,7 +21498,7 @@
       <c r="AP389" s="19"/>
       <c r="AQ389" s="19"/>
       <c r="AR389" s="22" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="390" spans="1:44" x14ac:dyDescent="0.25">
@@ -21483,7 +21546,7 @@
       <c r="AP390" s="19"/>
       <c r="AQ390" s="19"/>
       <c r="AR390" s="22" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="391" spans="1:44" x14ac:dyDescent="0.25">
@@ -21531,7 +21594,7 @@
       <c r="AP391" s="19"/>
       <c r="AQ391" s="19"/>
       <c r="AR391" s="22" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="392" spans="1:44" x14ac:dyDescent="0.25">
@@ -21579,7 +21642,7 @@
       <c r="AP392" s="19"/>
       <c r="AQ392" s="19"/>
       <c r="AR392" s="22" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="393" spans="1:44" x14ac:dyDescent="0.25">
@@ -21627,7 +21690,7 @@
       <c r="AP393" s="19"/>
       <c r="AQ393" s="19"/>
       <c r="AR393" s="22" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="394" spans="1:44" x14ac:dyDescent="0.25">
@@ -21675,7 +21738,7 @@
       <c r="AP394" s="19"/>
       <c r="AQ394" s="19"/>
       <c r="AR394" s="22" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="395" spans="1:44" x14ac:dyDescent="0.25">
@@ -21723,7 +21786,7 @@
       <c r="AP395" s="19"/>
       <c r="AQ395" s="19"/>
       <c r="AR395" s="22" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="396" spans="1:44" x14ac:dyDescent="0.25">
@@ -21771,7 +21834,7 @@
       <c r="AP396" s="19"/>
       <c r="AQ396" s="19"/>
       <c r="AR396" s="22" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="397" spans="1:44" x14ac:dyDescent="0.25">
@@ -21819,7 +21882,7 @@
       <c r="AP397" s="19"/>
       <c r="AQ397" s="19"/>
       <c r="AR397" s="22" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="398" spans="1:44" x14ac:dyDescent="0.25">
@@ -21867,7 +21930,7 @@
       <c r="AP398" s="19"/>
       <c r="AQ398" s="19"/>
       <c r="AR398" s="22" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="399" spans="1:44" x14ac:dyDescent="0.25">
@@ -21915,7 +21978,7 @@
       <c r="AP399" s="19"/>
       <c r="AQ399" s="19"/>
       <c r="AR399" s="22" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="400" spans="1:44" x14ac:dyDescent="0.25">
@@ -21963,7 +22026,7 @@
       <c r="AP400" s="19"/>
       <c r="AQ400" s="19"/>
       <c r="AR400" s="22" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="401" spans="1:44" x14ac:dyDescent="0.25">
@@ -22011,7 +22074,7 @@
       <c r="AP401" s="19"/>
       <c r="AQ401" s="19"/>
       <c r="AR401" s="22" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="402" spans="1:44" x14ac:dyDescent="0.25">
@@ -22059,7 +22122,7 @@
       <c r="AP402" s="19"/>
       <c r="AQ402" s="19"/>
       <c r="AR402" s="22" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="403" spans="1:44" x14ac:dyDescent="0.25">
@@ -22107,7 +22170,7 @@
       <c r="AP403" s="19"/>
       <c r="AQ403" s="19"/>
       <c r="AR403" s="22" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="404" spans="1:44" x14ac:dyDescent="0.25">
@@ -22155,7 +22218,7 @@
       <c r="AP404" s="19"/>
       <c r="AQ404" s="19"/>
       <c r="AR404" s="22" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="405" spans="1:44" x14ac:dyDescent="0.25">
@@ -22203,7 +22266,7 @@
       <c r="AP405" s="19"/>
       <c r="AQ405" s="19"/>
       <c r="AR405" s="22" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="406" spans="1:44" x14ac:dyDescent="0.25">
@@ -22251,7 +22314,7 @@
       <c r="AP406" s="19"/>
       <c r="AQ406" s="19"/>
       <c r="AR406" s="22" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="407" spans="1:44" x14ac:dyDescent="0.25">
@@ -22299,7 +22362,7 @@
       <c r="AP407" s="19"/>
       <c r="AQ407" s="19"/>
       <c r="AR407" s="22" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="408" spans="1:44" x14ac:dyDescent="0.25">
@@ -22347,7 +22410,7 @@
       <c r="AP408" s="19"/>
       <c r="AQ408" s="19"/>
       <c r="AR408" s="22" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="409" spans="1:44" x14ac:dyDescent="0.25">
@@ -22395,7 +22458,7 @@
       <c r="AP409" s="19"/>
       <c r="AQ409" s="19"/>
       <c r="AR409" s="22" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="410" spans="1:44" x14ac:dyDescent="0.25">
@@ -22443,7 +22506,7 @@
       <c r="AP410" s="19"/>
       <c r="AQ410" s="19"/>
       <c r="AR410" s="22" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="411" spans="1:44" x14ac:dyDescent="0.25">
@@ -22491,7 +22554,7 @@
       <c r="AP411" s="19"/>
       <c r="AQ411" s="19"/>
       <c r="AR411" s="22" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="412" spans="1:44" x14ac:dyDescent="0.25">
@@ -22539,7 +22602,7 @@
       <c r="AP412" s="19"/>
       <c r="AQ412" s="19"/>
       <c r="AR412" s="22" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="413" spans="1:44" x14ac:dyDescent="0.25">
@@ -22587,7 +22650,7 @@
       <c r="AP413" s="19"/>
       <c r="AQ413" s="19"/>
       <c r="AR413" s="22" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="414" spans="1:44" x14ac:dyDescent="0.25">
@@ -22635,7 +22698,7 @@
       <c r="AP414" s="19"/>
       <c r="AQ414" s="19"/>
       <c r="AR414" s="22" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="415" spans="1:44" x14ac:dyDescent="0.25">
@@ -22683,7 +22746,7 @@
       <c r="AP415" s="19"/>
       <c r="AQ415" s="19"/>
       <c r="AR415" s="22" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="416" spans="1:44" x14ac:dyDescent="0.25">
@@ -22731,7 +22794,7 @@
       <c r="AP416" s="19"/>
       <c r="AQ416" s="19"/>
       <c r="AR416" s="22" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="417" spans="1:44" x14ac:dyDescent="0.25">
@@ -22779,7 +22842,7 @@
       <c r="AP417" s="19"/>
       <c r="AQ417" s="19"/>
       <c r="AR417" s="22" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="418" spans="1:44" x14ac:dyDescent="0.25">
@@ -22827,7 +22890,7 @@
       <c r="AP418" s="19"/>
       <c r="AQ418" s="19"/>
       <c r="AR418" s="22" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="419" spans="1:44" x14ac:dyDescent="0.25">
@@ -22875,7 +22938,7 @@
       <c r="AP419" s="19"/>
       <c r="AQ419" s="19"/>
       <c r="AR419" s="22" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="420" spans="1:44" x14ac:dyDescent="0.25">
@@ -22923,7 +22986,7 @@
       <c r="AP420" s="19"/>
       <c r="AQ420" s="19"/>
       <c r="AR420" s="22" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="421" spans="1:44" x14ac:dyDescent="0.25">
@@ -22971,7 +23034,7 @@
       <c r="AP421" s="19"/>
       <c r="AQ421" s="19"/>
       <c r="AR421" s="22" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="422" spans="1:44" x14ac:dyDescent="0.25">
@@ -23019,7 +23082,7 @@
       <c r="AP422" s="19"/>
       <c r="AQ422" s="19"/>
       <c r="AR422" s="22" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="423" spans="1:44" x14ac:dyDescent="0.25">
@@ -23067,7 +23130,7 @@
       <c r="AP423" s="19"/>
       <c r="AQ423" s="19"/>
       <c r="AR423" s="22" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="424" spans="1:44" x14ac:dyDescent="0.25">
@@ -23115,7 +23178,7 @@
       <c r="AP424" s="19"/>
       <c r="AQ424" s="19"/>
       <c r="AR424" s="22" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="425" spans="1:44" x14ac:dyDescent="0.25">
@@ -23163,7 +23226,7 @@
       <c r="AP425" s="19"/>
       <c r="AQ425" s="19"/>
       <c r="AR425" s="22" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="426" spans="1:44" x14ac:dyDescent="0.25">
@@ -23211,7 +23274,7 @@
       <c r="AP426" s="19"/>
       <c r="AQ426" s="19"/>
       <c r="AR426" s="22" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="427" spans="1:44" x14ac:dyDescent="0.25">
@@ -23259,7 +23322,7 @@
       <c r="AP427" s="19"/>
       <c r="AQ427" s="19"/>
       <c r="AR427" s="22" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="428" spans="1:44" x14ac:dyDescent="0.25">
@@ -23307,7 +23370,7 @@
       <c r="AP428" s="19"/>
       <c r="AQ428" s="19"/>
       <c r="AR428" s="22" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="429" spans="1:44" x14ac:dyDescent="0.25">
@@ -23355,7 +23418,7 @@
       <c r="AP429" s="19"/>
       <c r="AQ429" s="19"/>
       <c r="AR429" s="22" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="430" spans="1:44" x14ac:dyDescent="0.25">
@@ -23403,7 +23466,7 @@
       <c r="AP430" s="19"/>
       <c r="AQ430" s="19"/>
       <c r="AR430" s="22" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="431" spans="1:44" x14ac:dyDescent="0.25">
@@ -23451,7 +23514,7 @@
       <c r="AP431" s="19"/>
       <c r="AQ431" s="19"/>
       <c r="AR431" s="22" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="432" spans="1:44" x14ac:dyDescent="0.25">
@@ -23499,7 +23562,7 @@
       <c r="AP432" s="19"/>
       <c r="AQ432" s="19"/>
       <c r="AR432" s="22" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="433" spans="1:44" x14ac:dyDescent="0.25">
@@ -23547,7 +23610,7 @@
       <c r="AP433" s="19"/>
       <c r="AQ433" s="19"/>
       <c r="AR433" s="22" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="434" spans="1:44" x14ac:dyDescent="0.25">
@@ -23595,7 +23658,7 @@
       <c r="AP434" s="19"/>
       <c r="AQ434" s="19"/>
       <c r="AR434" s="22" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="435" spans="1:44" x14ac:dyDescent="0.25">
@@ -23643,7 +23706,7 @@
       <c r="AP435" s="19"/>
       <c r="AQ435" s="19"/>
       <c r="AR435" s="22" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="436" spans="1:44" x14ac:dyDescent="0.25">
@@ -23691,7 +23754,7 @@
       <c r="AP436" s="19"/>
       <c r="AQ436" s="19"/>
       <c r="AR436" s="22" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="437" spans="1:44" x14ac:dyDescent="0.25">
@@ -23739,7 +23802,7 @@
       <c r="AP437" s="19"/>
       <c r="AQ437" s="19"/>
       <c r="AR437" s="22" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="438" spans="1:44" x14ac:dyDescent="0.25">
@@ -23787,7 +23850,7 @@
       <c r="AP438" s="19"/>
       <c r="AQ438" s="19"/>
       <c r="AR438" s="22" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="439" spans="1:44" x14ac:dyDescent="0.25">
@@ -23835,7 +23898,7 @@
       <c r="AP439" s="19"/>
       <c r="AQ439" s="19"/>
       <c r="AR439" s="22" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="440" spans="1:44" x14ac:dyDescent="0.25">
@@ -23883,7 +23946,7 @@
       <c r="AP440" s="19"/>
       <c r="AQ440" s="19"/>
       <c r="AR440" s="22" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="441" spans="1:44" x14ac:dyDescent="0.25">
@@ -23931,7 +23994,7 @@
       <c r="AP441" s="19"/>
       <c r="AQ441" s="19"/>
       <c r="AR441" s="22" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="442" spans="1:44" x14ac:dyDescent="0.25">
@@ -23979,7 +24042,7 @@
       <c r="AP442" s="19"/>
       <c r="AQ442" s="19"/>
       <c r="AR442" s="22" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="443" spans="1:44" x14ac:dyDescent="0.25">
@@ -24027,7 +24090,7 @@
       <c r="AP443" s="19"/>
       <c r="AQ443" s="19"/>
       <c r="AR443" s="22" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="444" spans="1:44" x14ac:dyDescent="0.25">
@@ -24075,7 +24138,7 @@
       <c r="AP444" s="19"/>
       <c r="AQ444" s="19"/>
       <c r="AR444" s="22" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="445" spans="1:44" x14ac:dyDescent="0.25">
@@ -24123,7 +24186,7 @@
       <c r="AP445" s="19"/>
       <c r="AQ445" s="19"/>
       <c r="AR445" s="22" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="446" spans="1:44" x14ac:dyDescent="0.25">
@@ -24171,7 +24234,7 @@
       <c r="AP446" s="19"/>
       <c r="AQ446" s="19"/>
       <c r="AR446" s="22" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="447" spans="1:44" x14ac:dyDescent="0.25">
@@ -24219,7 +24282,7 @@
       <c r="AP447" s="19"/>
       <c r="AQ447" s="19"/>
       <c r="AR447" s="22" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="448" spans="1:44" x14ac:dyDescent="0.25">
@@ -24267,7 +24330,7 @@
       <c r="AP448" s="19"/>
       <c r="AQ448" s="19"/>
       <c r="AR448" s="22" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="449" spans="1:44" x14ac:dyDescent="0.25">
@@ -24315,7 +24378,7 @@
       <c r="AP449" s="19"/>
       <c r="AQ449" s="19"/>
       <c r="AR449" s="22" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="450" spans="1:44" x14ac:dyDescent="0.25">
@@ -24363,7 +24426,7 @@
       <c r="AP450" s="19"/>
       <c r="AQ450" s="19"/>
       <c r="AR450" s="22" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="451" spans="1:44" x14ac:dyDescent="0.25">
@@ -24411,7 +24474,7 @@
       <c r="AP451" s="19"/>
       <c r="AQ451" s="19"/>
       <c r="AR451" s="22" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="452" spans="1:44" x14ac:dyDescent="0.25">
@@ -24459,7 +24522,7 @@
       <c r="AP452" s="19"/>
       <c r="AQ452" s="19"/>
       <c r="AR452" s="22" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="453" spans="1:44" x14ac:dyDescent="0.25">
@@ -24507,7 +24570,7 @@
       <c r="AP453" s="19"/>
       <c r="AQ453" s="19"/>
       <c r="AR453" s="22" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="454" spans="1:44" x14ac:dyDescent="0.25">
@@ -24555,7 +24618,7 @@
       <c r="AP454" s="19"/>
       <c r="AQ454" s="19"/>
       <c r="AR454" s="22" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="455" spans="1:44" x14ac:dyDescent="0.25">
@@ -24603,7 +24666,7 @@
       <c r="AP455" s="19"/>
       <c r="AQ455" s="19"/>
       <c r="AR455" s="22" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="456" spans="1:44" x14ac:dyDescent="0.25">
@@ -24651,7 +24714,7 @@
       <c r="AP456" s="19"/>
       <c r="AQ456" s="19"/>
       <c r="AR456" s="22" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="457" spans="1:44" x14ac:dyDescent="0.25">
@@ -24699,7 +24762,7 @@
       <c r="AP457" s="19"/>
       <c r="AQ457" s="19"/>
       <c r="AR457" s="22" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="458" spans="1:44" x14ac:dyDescent="0.25">
@@ -24747,7 +24810,7 @@
       <c r="AP458" s="19"/>
       <c r="AQ458" s="19"/>
       <c r="AR458" s="22" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="459" spans="1:44" x14ac:dyDescent="0.25">
@@ -24795,7 +24858,7 @@
       <c r="AP459" s="19"/>
       <c r="AQ459" s="19"/>
       <c r="AR459" s="22" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="460" spans="1:44" x14ac:dyDescent="0.25">
@@ -24843,7 +24906,7 @@
       <c r="AP460" s="19"/>
       <c r="AQ460" s="19"/>
       <c r="AR460" s="22" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="461" spans="1:44" x14ac:dyDescent="0.25">
@@ -24891,7 +24954,7 @@
       <c r="AP461" s="19"/>
       <c r="AQ461" s="19"/>
       <c r="AR461" s="22" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="462" spans="1:44" x14ac:dyDescent="0.25">
@@ -24939,7 +25002,7 @@
       <c r="AP462" s="19"/>
       <c r="AQ462" s="19"/>
       <c r="AR462" s="22" t="s">
-        <v>491</v>
+        <v>534</v>
       </c>
     </row>
     <row r="463" spans="1:44" x14ac:dyDescent="0.25">
@@ -24987,7 +25050,7 @@
       <c r="AP463" s="19"/>
       <c r="AQ463" s="19"/>
       <c r="AR463" s="22" t="s">
-        <v>492</v>
+        <v>537</v>
       </c>
     </row>
     <row r="464" spans="1:44" x14ac:dyDescent="0.25">
@@ -25035,11 +25098,14 @@
       <c r="AP464" s="19"/>
       <c r="AQ464" s="19"/>
       <c r="AR464" s="22" t="s">
-        <v>493</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:T1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A6"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="AA3" r:id="rId1"/>
     <hyperlink ref="AA7" r:id="rId2"/>

</xml_diff>

<commit_message>
titan Adjust for Holden testcase
</commit_message>
<xml_diff>
--- a/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
+++ b/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="540">
   <si>
     <t>TITAN</t>
   </si>
@@ -1683,6 +1683,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>HOLDEN</t>
   </si>
 </sst>
 </file>
@@ -2252,7 +2255,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,7 +2514,7 @@
         <v>523</v>
       </c>
       <c r="AE2" s="20" t="s">
-        <v>51</v>
+        <v>539</v>
       </c>
       <c r="AF2" s="20" t="s">
         <v>34</v>
@@ -2639,7 +2642,7 @@
         <v>523</v>
       </c>
       <c r="AE3" s="20" t="s">
-        <v>51</v>
+        <v>539</v>
       </c>
       <c r="AF3" s="20"/>
       <c r="AG3" s="20"/>
@@ -2761,7 +2764,7 @@
         <v>523</v>
       </c>
       <c r="AE4" s="20" t="s">
-        <v>51</v>
+        <v>539</v>
       </c>
       <c r="AF4" s="20"/>
       <c r="AG4" s="20"/>
@@ -2883,7 +2886,7 @@
         <v>523</v>
       </c>
       <c r="AE5" s="20" t="s">
-        <v>51</v>
+        <v>539</v>
       </c>
       <c r="AF5" s="20"/>
       <c r="AG5" s="20"/>
@@ -3005,7 +3008,7 @@
         <v>523</v>
       </c>
       <c r="AE6" s="20" t="s">
-        <v>51</v>
+        <v>539</v>
       </c>
       <c r="AF6" s="20"/>
       <c r="AG6" s="20"/>
@@ -3045,17 +3048,17 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="10" t="b">
-        <v>0</v>
+      <c r="B7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="D7" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="10" t="b">
-        <v>0</v>
+      <c r="E7" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="F7" s="10" t="b">
         <v>0</v>
@@ -3127,7 +3130,7 @@
         <v>523</v>
       </c>
       <c r="AE7" s="20" t="s">
-        <v>51</v>
+        <v>539</v>
       </c>
       <c r="AF7" s="20"/>
       <c r="AG7" s="20"/>

</xml_diff>

<commit_message>
CHANGE TRANSPORT OPTION METHOD
CHANGE VALIDATE FOR GET DETAIL BOOKING INTO ARRAY ROOT
</commit_message>
<xml_diff>
--- a/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
+++ b/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="539">
   <si>
     <t>TITAN</t>
   </si>
@@ -1652,9 +1652,6 @@
     <t>VN</t>
   </si>
   <si>
-    <t>NOTEXIST</t>
-  </si>
-  <si>
     <t>NEW</t>
   </si>
   <si>
@@ -1683,6 +1680,9 @@
   </si>
   <si>
     <t>FIAT</t>
+  </si>
+  <si>
+    <t>DEMO</t>
   </si>
 </sst>
 </file>
@@ -1884,7 +1884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1962,6 +1962,9 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1969,6 +1972,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0066"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2252,7 +2260,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2457,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>21</v>
@@ -2505,13 +2513,13 @@
         <v>19</v>
       </c>
       <c r="AC2" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AD2" s="20" t="s">
         <v>521</v>
       </c>
       <c r="AE2" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AF2" s="20" t="s">
         <v>33</v>
@@ -2555,7 +2563,7 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B3" s="6" t="b">
         <v>1</v>
@@ -2591,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>21</v>
@@ -2600,7 +2608,7 @@
         <v>21</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q3" s="20"/>
       <c r="R3" s="20"/>
@@ -2630,16 +2638,16 @@
         <v>526</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AC3" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AD3" s="20" t="s">
         <v>521</v>
       </c>
       <c r="AE3" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AF3" s="20"/>
       <c r="AG3" s="20"/>
@@ -2674,7 +2682,7 @@
         <v>18</v>
       </c>
       <c r="AR3" s="22" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
@@ -2713,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>21</v>
@@ -2722,7 +2730,7 @@
         <v>21</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
@@ -2752,16 +2760,16 @@
         <v>526</v>
       </c>
       <c r="AB4" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AC4" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AD4" s="20" t="s">
         <v>521</v>
       </c>
       <c r="AE4" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AF4" s="20"/>
       <c r="AG4" s="20"/>
@@ -2778,7 +2786,7 @@
         <v>20</v>
       </c>
       <c r="AL4" s="11" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AM4" s="10" t="b">
         <v>0</v>
@@ -2835,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>21</v>
@@ -2844,7 +2852,7 @@
         <v>21</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q5" s="20"/>
       <c r="R5" s="20"/>
@@ -2874,16 +2882,16 @@
         <v>526</v>
       </c>
       <c r="AB5" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AC5" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AD5" s="20" t="s">
         <v>521</v>
       </c>
       <c r="AE5" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AF5" s="20"/>
       <c r="AG5" s="20"/>
@@ -2957,7 +2965,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>21</v>
@@ -2966,7 +2974,7 @@
         <v>21</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="20"/>
@@ -2996,16 +3004,16 @@
         <v>526</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AC6" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AD6" s="20" t="s">
         <v>521</v>
       </c>
       <c r="AE6" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AF6" s="20"/>
       <c r="AG6" s="20"/>
@@ -3022,7 +3030,7 @@
         <v>21</v>
       </c>
       <c r="AL6" s="11" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AM6" s="10" t="b">
         <v>0</v>
@@ -3044,21 +3052,23 @@
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="6" t="b">
+      <c r="A7" s="29" t="s">
+        <v>538</v>
+      </c>
+      <c r="B7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6" t="b">
         <v>1</v>
-      </c>
-      <c r="C7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="10" t="b">
-        <v>0</v>
       </c>
       <c r="G7" s="10" t="b">
         <v>0</v>
@@ -3066,11 +3076,11 @@
       <c r="H7" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="10" t="b">
-        <v>0</v>
+      <c r="I7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="K7" s="10" t="b">
         <v>0</v>
@@ -3079,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>21</v>
@@ -3088,7 +3098,7 @@
         <v>21</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="20"/>
@@ -3118,16 +3128,16 @@
         <v>526</v>
       </c>
       <c r="AB7" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AC7" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AD7" s="20" t="s">
         <v>521</v>
       </c>
       <c r="AE7" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AF7" s="20"/>
       <c r="AG7" s="20"/>
@@ -3138,7 +3148,7 @@
         <v>36</v>
       </c>
       <c r="AJ7" s="10" t="s">
-        <v>528</v>
+        <v>18</v>
       </c>
       <c r="AK7" s="11" t="s">
         <v>21</v>
@@ -25002,7 +25012,7 @@
       <c r="AP462" s="19"/>
       <c r="AQ462" s="19"/>
       <c r="AR462" s="22" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="463" spans="1:44" x14ac:dyDescent="0.25">
@@ -25050,7 +25060,7 @@
       <c r="AP463" s="19"/>
       <c r="AQ463" s="19"/>
       <c r="AR463" s="22" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="464" spans="1:44" x14ac:dyDescent="0.25">
@@ -25098,7 +25108,7 @@
       <c r="AP464" s="19"/>
       <c r="AQ464" s="19"/>
       <c r="AR464" s="22" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -25108,10 +25118,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AA3" r:id="rId1"/>
-    <hyperlink ref="AA7" r:id="rId2"/>
-    <hyperlink ref="AA4" r:id="rId3"/>
-    <hyperlink ref="AA5" r:id="rId4"/>
-    <hyperlink ref="AA6" r:id="rId5"/>
+    <hyperlink ref="AA4" r:id="rId2"/>
+    <hyperlink ref="AA5" r:id="rId3"/>
+    <hyperlink ref="AA6" r:id="rId4"/>
+    <hyperlink ref="AA7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>